<commit_message>
EJERCICIOS 3 al 11 terminados
</commit_message>
<xml_diff>
--- a/MATRICES/matrices.xlsx
+++ b/MATRICES/matrices.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\serve\ARCHIVOS VARIOS\python-exercises\MATRICES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DF8EA50-6C9F-487E-958C-4E46EB838D85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF053F73-560A-4AF7-BDA5-FDD06361AB0C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26055" yWindow="1380" windowWidth="15375" windowHeight="7785" xr2:uid="{D8BD301B-0896-44DD-B534-8AC196178EBF}"/>
+    <workbookView xWindow="5115" yWindow="3015" windowWidth="15375" windowHeight="7785" xr2:uid="{D8BD301B-0896-44DD-B534-8AC196178EBF}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="51">
   <si>
     <t>00</t>
   </si>
@@ -208,7 +208,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -218,6 +218,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -234,7 +240,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -245,6 +251,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -561,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{124D0BB0-B589-4BBF-89A0-F5133410D80B}">
-  <dimension ref="A1:J167"/>
+  <dimension ref="A1:J176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="192" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A98" sqref="A98:G98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1129,73 +1138,171 @@
       <c r="H30" s="1"/>
     </row>
     <row r="31" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
+      <c r="A31" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="H31" s="1"/>
     </row>
     <row r="32" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
+      <c r="A32" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="H32" s="1"/>
     </row>
     <row r="33" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
+      <c r="A33" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="H33" s="1"/>
     </row>
     <row r="34" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
+      <c r="A34" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>33</v>
+      </c>
       <c r="H34" s="1"/>
     </row>
     <row r="35" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
+      <c r="A35" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="H35" s="1"/>
     </row>
     <row r="36" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
+      <c r="A36" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H36" s="1"/>
     </row>
     <row r="37" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
+      <c r="A37" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="H37" s="1"/>
     </row>
     <row r="38" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1218,7 +1325,7 @@
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
     </row>
-    <row r="40" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -1228,77 +1335,175 @@
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
     </row>
-    <row r="41" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
+    <row r="41" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="H41" s="1"/>
     </row>
-    <row r="42" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
+    <row r="42" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>13</v>
+      </c>
       <c r="H42" s="1"/>
     </row>
-    <row r="43" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
+    <row r="43" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G43" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="H43" s="1"/>
     </row>
-    <row r="44" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="1"/>
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
+    <row r="44" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G44" s="5" t="s">
+        <v>33</v>
+      </c>
       <c r="H44" s="1"/>
     </row>
-    <row r="45" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
-      <c r="E45" s="1"/>
-      <c r="F45" s="1"/>
-      <c r="G45" s="1"/>
+    <row r="45" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G45" s="5" t="s">
+        <v>38</v>
+      </c>
       <c r="H45" s="1"/>
     </row>
-    <row r="46" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
-      <c r="G46" s="1"/>
+    <row r="46" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G46" s="5" t="s">
+        <v>43</v>
+      </c>
       <c r="H46" s="1"/>
     </row>
-    <row r="47" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="1"/>
-      <c r="B47" s="1"/>
-      <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
-      <c r="E47" s="1"/>
-      <c r="F47" s="1"/>
-      <c r="G47" s="1"/>
+    <row r="47" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G47" s="5" t="s">
+        <v>30</v>
+      </c>
       <c r="H47" s="1"/>
     </row>
-    <row r="48" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -1308,7 +1513,7 @@
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
     </row>
-    <row r="49" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -1318,7 +1523,7 @@
       <c r="G49" s="1"/>
       <c r="H49" s="1"/>
     </row>
-    <row r="50" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -1328,77 +1533,175 @@
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
     </row>
-    <row r="51" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="1"/>
-      <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
-      <c r="D51" s="1"/>
-      <c r="E51" s="1"/>
-      <c r="F51" s="1"/>
-      <c r="G51" s="1"/>
+    <row r="51" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G51" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="H51" s="1"/>
     </row>
-    <row r="52" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="1"/>
-      <c r="B52" s="1"/>
-      <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
-      <c r="F52" s="1"/>
-      <c r="G52" s="1"/>
+    <row r="52" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G52" s="5" t="s">
+        <v>13</v>
+      </c>
       <c r="H52" s="1"/>
     </row>
-    <row r="53" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="1"/>
-      <c r="B53" s="1"/>
-      <c r="C53" s="1"/>
-      <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
-      <c r="G53" s="1"/>
+    <row r="53" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E53" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F53" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G53" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="H53" s="1"/>
     </row>
-    <row r="54" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="1"/>
-      <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
-      <c r="D54" s="1"/>
-      <c r="E54" s="1"/>
-      <c r="F54" s="1"/>
-      <c r="G54" s="1"/>
+    <row r="54" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G54" s="5" t="s">
+        <v>33</v>
+      </c>
       <c r="H54" s="1"/>
     </row>
-    <row r="55" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="1"/>
-      <c r="B55" s="1"/>
-      <c r="C55" s="1"/>
-      <c r="D55" s="1"/>
-      <c r="E55" s="1"/>
-      <c r="F55" s="1"/>
-      <c r="G55" s="1"/>
+    <row r="55" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G55" s="5" t="s">
+        <v>38</v>
+      </c>
       <c r="H55" s="1"/>
     </row>
-    <row r="56" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="1"/>
-      <c r="B56" s="1"/>
-      <c r="C56" s="1"/>
-      <c r="D56" s="1"/>
-      <c r="E56" s="1"/>
-      <c r="F56" s="1"/>
-      <c r="G56" s="1"/>
+    <row r="56" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G56" s="5" t="s">
+        <v>43</v>
+      </c>
       <c r="H56" s="1"/>
     </row>
-    <row r="57" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="1"/>
-      <c r="B57" s="1"/>
-      <c r="C57" s="1"/>
-      <c r="D57" s="1"/>
-      <c r="E57" s="1"/>
-      <c r="F57" s="1"/>
-      <c r="G57" s="1"/>
+    <row r="57" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G57" s="5" t="s">
+        <v>30</v>
+      </c>
       <c r="H57" s="1"/>
     </row>
-    <row r="58" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -1408,7 +1711,7 @@
       <c r="G58" s="1"/>
       <c r="H58" s="1"/>
     </row>
-    <row r="59" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -1418,7 +1721,7 @@
       <c r="G59" s="1"/>
       <c r="H59" s="1"/>
     </row>
-    <row r="60" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -1428,77 +1731,175 @@
       <c r="G60" s="1"/>
       <c r="H60" s="1"/>
     </row>
-    <row r="61" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="1"/>
-      <c r="B61" s="1"/>
-      <c r="C61" s="1"/>
-      <c r="D61" s="1"/>
-      <c r="E61" s="1"/>
-      <c r="F61" s="1"/>
-      <c r="G61" s="1"/>
+    <row r="61" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E61" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F61" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G61" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="H61" s="1"/>
     </row>
-    <row r="62" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="1"/>
-      <c r="B62" s="1"/>
-      <c r="C62" s="1"/>
-      <c r="D62" s="1"/>
-      <c r="E62" s="1"/>
-      <c r="F62" s="1"/>
-      <c r="G62" s="1"/>
+    <row r="62" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E62" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F62" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G62" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="H62" s="1"/>
     </row>
-    <row r="63" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="1"/>
-      <c r="B63" s="1"/>
-      <c r="C63" s="1"/>
-      <c r="D63" s="1"/>
-      <c r="E63" s="1"/>
-      <c r="F63" s="1"/>
-      <c r="G63" s="1"/>
+    <row r="63" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E63" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G63" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="H63" s="1"/>
     </row>
-    <row r="64" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="1"/>
-      <c r="B64" s="1"/>
-      <c r="C64" s="1"/>
-      <c r="D64" s="1"/>
-      <c r="E64" s="1"/>
-      <c r="F64" s="1"/>
-      <c r="G64" s="1"/>
+    <row r="64" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F64" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G64" s="3" t="s">
+        <v>33</v>
+      </c>
       <c r="H64" s="1"/>
     </row>
-    <row r="65" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="1"/>
-      <c r="B65" s="1"/>
-      <c r="C65" s="1"/>
-      <c r="D65" s="1"/>
-      <c r="E65" s="1"/>
-      <c r="F65" s="1"/>
-      <c r="G65" s="1"/>
+    <row r="65" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F65" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G65" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="H65" s="1"/>
     </row>
-    <row r="66" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="1"/>
-      <c r="B66" s="1"/>
-      <c r="C66" s="1"/>
-      <c r="D66" s="1"/>
-      <c r="E66" s="1"/>
-      <c r="F66" s="1"/>
-      <c r="G66" s="1"/>
+    <row r="66" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E66" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F66" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G66" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H66" s="1"/>
     </row>
-    <row r="67" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="1"/>
-      <c r="B67" s="1"/>
-      <c r="C67" s="1"/>
-      <c r="D67" s="1"/>
-      <c r="E67" s="1"/>
-      <c r="F67" s="1"/>
-      <c r="G67" s="1"/>
+    <row r="67" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E67" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F67" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G67" s="5" t="s">
+        <v>30</v>
+      </c>
       <c r="H67" s="1"/>
     </row>
-    <row r="68" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -1508,77 +1909,175 @@
       <c r="G68" s="1"/>
       <c r="H68" s="1"/>
     </row>
-    <row r="69" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="1"/>
-      <c r="B69" s="1"/>
-      <c r="C69" s="1"/>
-      <c r="D69" s="1"/>
-      <c r="E69" s="1"/>
-      <c r="F69" s="1"/>
-      <c r="G69" s="1"/>
+    <row r="69" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E69" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F69" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G69" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="H69" s="1"/>
     </row>
-    <row r="70" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="1"/>
-      <c r="B70" s="1"/>
-      <c r="C70" s="1"/>
-      <c r="D70" s="1"/>
-      <c r="E70" s="1"/>
-      <c r="F70" s="1"/>
-      <c r="G70" s="1"/>
+    <row r="70" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C70" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E70" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F70" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G70" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="H70" s="1"/>
     </row>
-    <row r="71" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="1"/>
-      <c r="B71" s="1"/>
-      <c r="C71" s="1"/>
-      <c r="D71" s="1"/>
-      <c r="E71" s="1"/>
-      <c r="F71" s="1"/>
-      <c r="G71" s="1"/>
+    <row r="71" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C71" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D71" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F71" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G71" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="H71" s="1"/>
     </row>
-    <row r="72" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="1"/>
-      <c r="B72" s="1"/>
-      <c r="C72" s="1"/>
-      <c r="D72" s="1"/>
-      <c r="E72" s="1"/>
-      <c r="F72" s="1"/>
-      <c r="G72" s="1"/>
+    <row r="72" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C72" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E72" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F72" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G72" s="3" t="s">
+        <v>33</v>
+      </c>
       <c r="H72" s="1"/>
     </row>
-    <row r="73" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="1"/>
-      <c r="B73" s="1"/>
-      <c r="C73" s="1"/>
-      <c r="D73" s="1"/>
-      <c r="E73" s="1"/>
-      <c r="F73" s="1"/>
-      <c r="G73" s="1"/>
+    <row r="73" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F73" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G73" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="H73" s="1"/>
     </row>
-    <row r="74" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="1"/>
-      <c r="B74" s="1"/>
-      <c r="C74" s="1"/>
-      <c r="D74" s="1"/>
-      <c r="E74" s="1"/>
-      <c r="F74" s="1"/>
-      <c r="G74" s="1"/>
+    <row r="74" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F74" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G74" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H74" s="1"/>
     </row>
-    <row r="75" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="1"/>
-      <c r="B75" s="1"/>
-      <c r="C75" s="1"/>
-      <c r="D75" s="1"/>
-      <c r="E75" s="1"/>
-      <c r="F75" s="1"/>
-      <c r="G75" s="1"/>
+    <row r="75" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E75" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F75" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G75" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="H75" s="1"/>
     </row>
-    <row r="76" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -1588,7 +2087,7 @@
       <c r="G76" s="1"/>
       <c r="H76" s="1"/>
     </row>
-    <row r="77" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -1598,77 +2097,175 @@
       <c r="G77" s="1"/>
       <c r="H77" s="1"/>
     </row>
-    <row r="78" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="1"/>
-      <c r="B78" s="1"/>
-      <c r="C78" s="1"/>
-      <c r="D78" s="1"/>
-      <c r="E78" s="1"/>
-      <c r="F78" s="1"/>
-      <c r="G78" s="1"/>
+    <row r="78" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B78" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C78" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D78" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E78" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F78" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G78" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="H78" s="1"/>
     </row>
-    <row r="79" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="1"/>
-      <c r="B79" s="1"/>
-      <c r="C79" s="1"/>
-      <c r="D79" s="1"/>
-      <c r="E79" s="1"/>
-      <c r="F79" s="1"/>
-      <c r="G79" s="1"/>
+    <row r="79" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B79" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C79" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D79" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E79" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F79" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G79" s="6" t="s">
+        <v>13</v>
+      </c>
       <c r="H79" s="1"/>
     </row>
-    <row r="80" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="1"/>
-      <c r="B80" s="1"/>
-      <c r="C80" s="1"/>
-      <c r="D80" s="1"/>
-      <c r="E80" s="1"/>
-      <c r="F80" s="1"/>
-      <c r="G80" s="1"/>
+    <row r="80" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B80" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C80" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D80" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E80" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F80" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G80" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="H80" s="1"/>
     </row>
-    <row r="81" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="1"/>
-      <c r="B81" s="1"/>
-      <c r="C81" s="1"/>
-      <c r="D81" s="1"/>
-      <c r="E81" s="1"/>
-      <c r="F81" s="1"/>
-      <c r="G81" s="1"/>
+    <row r="81" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B81" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C81" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D81" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E81" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F81" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G81" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="H81" s="1"/>
     </row>
-    <row r="82" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="1"/>
-      <c r="B82" s="1"/>
-      <c r="C82" s="1"/>
-      <c r="D82" s="1"/>
-      <c r="E82" s="1"/>
-      <c r="F82" s="1"/>
-      <c r="G82" s="1"/>
+    <row r="82" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B82" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C82" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D82" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E82" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F82" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G82" s="5" t="s">
+        <v>38</v>
+      </c>
       <c r="H82" s="1"/>
     </row>
-    <row r="83" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="1"/>
-      <c r="B83" s="1"/>
-      <c r="C83" s="1"/>
-      <c r="D83" s="1"/>
-      <c r="E83" s="1"/>
-      <c r="F83" s="1"/>
-      <c r="G83" s="1"/>
+    <row r="83" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B83" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C83" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D83" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E83" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F83" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G83" s="6" t="s">
+        <v>43</v>
+      </c>
       <c r="H83" s="1"/>
     </row>
-    <row r="84" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="1"/>
-      <c r="B84" s="1"/>
-      <c r="C84" s="1"/>
-      <c r="D84" s="1"/>
-      <c r="E84" s="1"/>
-      <c r="F84" s="1"/>
-      <c r="G84" s="1"/>
+    <row r="84" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B84" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C84" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D84" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E84" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F84" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G84" s="5" t="s">
+        <v>30</v>
+      </c>
       <c r="H84" s="1"/>
     </row>
-    <row r="85" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -1678,7 +2275,7 @@
       <c r="G85" s="1"/>
       <c r="H85" s="1"/>
     </row>
-    <row r="86" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -1688,7 +2285,7 @@
       <c r="G86" s="1"/>
       <c r="H86" s="1"/>
     </row>
-    <row r="87" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -1698,77 +2295,175 @@
       <c r="G87" s="1"/>
       <c r="H87" s="1"/>
     </row>
-    <row r="88" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="1"/>
-      <c r="B88" s="1"/>
-      <c r="C88" s="1"/>
-      <c r="D88" s="1"/>
-      <c r="E88" s="1"/>
-      <c r="F88" s="1"/>
-      <c r="G88" s="1"/>
+    <row r="88" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B88" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C88" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D88" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E88" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F88" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G88" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="H88" s="1"/>
     </row>
-    <row r="89" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="1"/>
-      <c r="B89" s="1"/>
-      <c r="C89" s="1"/>
-      <c r="D89" s="1"/>
-      <c r="E89" s="1"/>
-      <c r="F89" s="1"/>
-      <c r="G89" s="1"/>
+    <row r="89" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B89" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C89" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D89" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E89" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F89" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G89" s="5" t="s">
+        <v>13</v>
+      </c>
       <c r="H89" s="1"/>
     </row>
-    <row r="90" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="1"/>
-      <c r="B90" s="1"/>
-      <c r="C90" s="1"/>
-      <c r="D90" s="1"/>
-      <c r="E90" s="1"/>
-      <c r="F90" s="1"/>
-      <c r="G90" s="1"/>
+    <row r="90" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B90" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C90" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D90" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E90" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F90" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G90" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="H90" s="1"/>
     </row>
-    <row r="91" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="1"/>
-      <c r="B91" s="1"/>
-      <c r="C91" s="1"/>
-      <c r="D91" s="1"/>
-      <c r="E91" s="1"/>
-      <c r="F91" s="1"/>
-      <c r="G91" s="1"/>
+    <row r="91" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B91" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C91" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E91" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F91" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G91" s="5" t="s">
+        <v>33</v>
+      </c>
       <c r="H91" s="1"/>
     </row>
-    <row r="92" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="1"/>
-      <c r="B92" s="1"/>
-      <c r="C92" s="1"/>
-      <c r="D92" s="1"/>
-      <c r="E92" s="1"/>
-      <c r="F92" s="1"/>
-      <c r="G92" s="1"/>
+    <row r="92" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B92" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D92" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E92" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F92" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G92" s="5" t="s">
+        <v>38</v>
+      </c>
       <c r="H92" s="1"/>
     </row>
-    <row r="93" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="1"/>
-      <c r="B93" s="1"/>
-      <c r="C93" s="1"/>
-      <c r="D93" s="1"/>
-      <c r="E93" s="1"/>
-      <c r="F93" s="1"/>
-      <c r="G93" s="1"/>
+    <row r="93" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C93" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D93" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E93" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F93" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G93" s="5" t="s">
+        <v>43</v>
+      </c>
       <c r="H93" s="1"/>
     </row>
-    <row r="94" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="1"/>
-      <c r="B94" s="1"/>
-      <c r="C94" s="1"/>
-      <c r="D94" s="1"/>
-      <c r="E94" s="1"/>
-      <c r="F94" s="1"/>
-      <c r="G94" s="1"/>
+    <row r="94" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B94" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C94" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D94" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E94" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F94" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G94" s="5" t="s">
+        <v>30</v>
+      </c>
       <c r="H94" s="1"/>
     </row>
-    <row r="95" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -1778,7 +2473,7 @@
       <c r="G95" s="1"/>
       <c r="H95" s="1"/>
     </row>
-    <row r="96" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -1788,7 +2483,7 @@
       <c r="G96" s="1"/>
       <c r="H96" s="1"/>
     </row>
-    <row r="97" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -1798,77 +2493,175 @@
       <c r="G97" s="1"/>
       <c r="H97" s="1"/>
     </row>
-    <row r="98" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="1"/>
-      <c r="B98" s="1"/>
-      <c r="C98" s="1"/>
-      <c r="D98" s="1"/>
-      <c r="E98" s="1"/>
-      <c r="F98" s="1"/>
-      <c r="G98" s="1"/>
+    <row r="98" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B98" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C98" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D98" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E98" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F98" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G98" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="H98" s="1"/>
     </row>
-    <row r="99" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="1"/>
-      <c r="B99" s="1"/>
-      <c r="C99" s="1"/>
-      <c r="D99" s="1"/>
-      <c r="E99" s="1"/>
-      <c r="F99" s="1"/>
-      <c r="G99" s="1"/>
+    <row r="99" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B99" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C99" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D99" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E99" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F99" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G99" s="5" t="s">
+        <v>13</v>
+      </c>
       <c r="H99" s="1"/>
     </row>
-    <row r="100" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="1"/>
-      <c r="B100" s="1"/>
-      <c r="C100" s="1"/>
-      <c r="D100" s="1"/>
-      <c r="E100" s="1"/>
-      <c r="F100" s="1"/>
-      <c r="G100" s="1"/>
+    <row r="100" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B100" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C100" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D100" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E100" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F100" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G100" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="H100" s="1"/>
     </row>
-    <row r="101" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="1"/>
-      <c r="B101" s="1"/>
-      <c r="C101" s="1"/>
-      <c r="D101" s="1"/>
-      <c r="E101" s="1"/>
-      <c r="F101" s="1"/>
-      <c r="G101" s="1"/>
+    <row r="101" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B101" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C101" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D101" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E101" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F101" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G101" s="5" t="s">
+        <v>33</v>
+      </c>
       <c r="H101" s="1"/>
     </row>
-    <row r="102" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="1"/>
-      <c r="B102" s="1"/>
-      <c r="C102" s="1"/>
-      <c r="D102" s="1"/>
-      <c r="E102" s="1"/>
-      <c r="F102" s="1"/>
-      <c r="G102" s="1"/>
+    <row r="102" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B102" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C102" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D102" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E102" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F102" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G102" s="5" t="s">
+        <v>38</v>
+      </c>
       <c r="H102" s="1"/>
     </row>
-    <row r="103" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="1"/>
-      <c r="B103" s="1"/>
-      <c r="C103" s="1"/>
-      <c r="D103" s="1"/>
-      <c r="E103" s="1"/>
-      <c r="F103" s="1"/>
-      <c r="G103" s="1"/>
+    <row r="103" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B103" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C103" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D103" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E103" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F103" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G103" s="5" t="s">
+        <v>43</v>
+      </c>
       <c r="H103" s="1"/>
     </row>
-    <row r="104" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="1"/>
-      <c r="B104" s="1"/>
-      <c r="C104" s="1"/>
-      <c r="D104" s="1"/>
-      <c r="E104" s="1"/>
-      <c r="F104" s="1"/>
-      <c r="G104" s="1"/>
+    <row r="104" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B104" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C104" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D104" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E104" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F104" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G104" s="5" t="s">
+        <v>30</v>
+      </c>
       <c r="H104" s="1"/>
     </row>
-    <row r="105" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
@@ -1878,7 +2671,7 @@
       <c r="G105" s="1"/>
       <c r="H105" s="1"/>
     </row>
-    <row r="106" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
@@ -1888,7 +2681,7 @@
       <c r="G106" s="1"/>
       <c r="H106" s="1"/>
     </row>
-    <row r="107" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
@@ -1898,7 +2691,7 @@
       <c r="G107" s="1"/>
       <c r="H107" s="1"/>
     </row>
-    <row r="108" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
@@ -1908,7 +2701,7 @@
       <c r="G108" s="1"/>
       <c r="H108" s="1"/>
     </row>
-    <row r="109" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
@@ -1918,7 +2711,7 @@
       <c r="G109" s="1"/>
       <c r="H109" s="1"/>
     </row>
-    <row r="110" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
@@ -1928,7 +2721,7 @@
       <c r="G110" s="1"/>
       <c r="H110" s="1"/>
     </row>
-    <row r="111" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
@@ -1938,7 +2731,7 @@
       <c r="G111" s="1"/>
       <c r="H111" s="1"/>
     </row>
-    <row r="112" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
@@ -1948,7 +2741,7 @@
       <c r="G112" s="1"/>
       <c r="H112" s="1"/>
     </row>
-    <row r="113" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
@@ -1958,7 +2751,7 @@
       <c r="G113" s="1"/>
       <c r="H113" s="1"/>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
@@ -1968,7 +2761,7 @@
       <c r="G114" s="1"/>
       <c r="H114" s="1"/>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
@@ -1978,7 +2771,7 @@
       <c r="G115" s="1"/>
       <c r="H115" s="1"/>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
@@ -1988,7 +2781,7 @@
       <c r="G116" s="1"/>
       <c r="H116" s="1"/>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
@@ -1998,7 +2791,7 @@
       <c r="G117" s="1"/>
       <c r="H117" s="1"/>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
@@ -2008,7 +2801,7 @@
       <c r="G118" s="1"/>
       <c r="H118" s="1"/>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
@@ -2018,7 +2811,7 @@
       <c r="G119" s="1"/>
       <c r="H119" s="1"/>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
@@ -2028,7 +2821,7 @@
       <c r="G120" s="1"/>
       <c r="H120" s="1"/>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
@@ -2038,7 +2831,7 @@
       <c r="G121" s="1"/>
       <c r="H121" s="1"/>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="1"/>
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
@@ -2048,7 +2841,7 @@
       <c r="G122" s="1"/>
       <c r="H122" s="1"/>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="1"/>
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
@@ -2058,7 +2851,7 @@
       <c r="G123" s="1"/>
       <c r="H123" s="1"/>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="1"/>
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
@@ -2068,7 +2861,7 @@
       <c r="G124" s="1"/>
       <c r="H124" s="1"/>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="1"/>
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
@@ -2078,7 +2871,7 @@
       <c r="G125" s="1"/>
       <c r="H125" s="1"/>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="1"/>
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
@@ -2088,7 +2881,7 @@
       <c r="G126" s="1"/>
       <c r="H126" s="1"/>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="1"/>
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
@@ -2098,7 +2891,7 @@
       <c r="G127" s="1"/>
       <c r="H127" s="1"/>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="1"/>
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
@@ -2108,7 +2901,7 @@
       <c r="G128" s="1"/>
       <c r="H128" s="1"/>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="1"/>
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
@@ -2118,7 +2911,7 @@
       <c r="G129" s="1"/>
       <c r="H129" s="1"/>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="1"/>
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
@@ -2128,7 +2921,7 @@
       <c r="G130" s="1"/>
       <c r="H130" s="1"/>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="1"/>
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
@@ -2138,7 +2931,7 @@
       <c r="G131" s="1"/>
       <c r="H131" s="1"/>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="1"/>
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
@@ -2148,7 +2941,7 @@
       <c r="G132" s="1"/>
       <c r="H132" s="1"/>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="1"/>
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
@@ -2158,7 +2951,7 @@
       <c r="G133" s="1"/>
       <c r="H133" s="1"/>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="1"/>
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
@@ -2168,7 +2961,7 @@
       <c r="G134" s="1"/>
       <c r="H134" s="1"/>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="1"/>
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
@@ -2178,7 +2971,7 @@
       <c r="G135" s="1"/>
       <c r="H135" s="1"/>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="1"/>
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
@@ -2188,7 +2981,7 @@
       <c r="G136" s="1"/>
       <c r="H136" s="1"/>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="1"/>
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
@@ -2198,7 +2991,7 @@
       <c r="G137" s="1"/>
       <c r="H137" s="1"/>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="1"/>
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
@@ -2208,7 +3001,7 @@
       <c r="G138" s="1"/>
       <c r="H138" s="1"/>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="1"/>
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
@@ -2218,7 +3011,7 @@
       <c r="G139" s="1"/>
       <c r="H139" s="1"/>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="1"/>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
@@ -2228,7 +3021,7 @@
       <c r="G140" s="1"/>
       <c r="H140" s="1"/>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="1"/>
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
@@ -2238,7 +3031,7 @@
       <c r="G141" s="1"/>
       <c r="H141" s="1"/>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="1"/>
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
@@ -2248,7 +3041,7 @@
       <c r="G142" s="1"/>
       <c r="H142" s="1"/>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="1"/>
       <c r="B143" s="1"/>
       <c r="C143" s="1"/>
@@ -2258,7 +3051,7 @@
       <c r="G143" s="1"/>
       <c r="H143" s="1"/>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="1"/>
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
@@ -2268,7 +3061,7 @@
       <c r="G144" s="1"/>
       <c r="H144" s="1"/>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="1"/>
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
@@ -2278,7 +3071,7 @@
       <c r="G145" s="1"/>
       <c r="H145" s="1"/>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="1"/>
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
@@ -2288,7 +3081,7 @@
       <c r="G146" s="1"/>
       <c r="H146" s="1"/>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="1"/>
       <c r="B147" s="1"/>
       <c r="C147" s="1"/>
@@ -2298,7 +3091,7 @@
       <c r="G147" s="1"/>
       <c r="H147" s="1"/>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="1"/>
       <c r="B148" s="1"/>
       <c r="C148" s="1"/>
@@ -2308,7 +3101,7 @@
       <c r="G148" s="1"/>
       <c r="H148" s="1"/>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="1"/>
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
@@ -2318,7 +3111,7 @@
       <c r="G149" s="1"/>
       <c r="H149" s="1"/>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="1"/>
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
@@ -2328,7 +3121,7 @@
       <c r="G150" s="1"/>
       <c r="H150" s="1"/>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="1"/>
       <c r="B151" s="1"/>
       <c r="C151" s="1"/>
@@ -2338,7 +3131,7 @@
       <c r="G151" s="1"/>
       <c r="H151" s="1"/>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="1"/>
       <c r="B152" s="1"/>
       <c r="C152" s="1"/>
@@ -2348,7 +3141,7 @@
       <c r="G152" s="1"/>
       <c r="H152" s="1"/>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="1"/>
       <c r="B153" s="1"/>
       <c r="C153" s="1"/>
@@ -2358,7 +3151,7 @@
       <c r="G153" s="1"/>
       <c r="H153" s="1"/>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="1"/>
       <c r="B154" s="1"/>
       <c r="C154" s="1"/>
@@ -2368,7 +3161,7 @@
       <c r="G154" s="1"/>
       <c r="H154" s="1"/>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="1"/>
       <c r="B155" s="1"/>
       <c r="C155" s="1"/>
@@ -2378,7 +3171,7 @@
       <c r="G155" s="1"/>
       <c r="H155" s="1"/>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="1"/>
       <c r="B156" s="1"/>
       <c r="C156" s="1"/>
@@ -2388,7 +3181,7 @@
       <c r="G156" s="1"/>
       <c r="H156" s="1"/>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="1"/>
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
@@ -2398,7 +3191,7 @@
       <c r="G157" s="1"/>
       <c r="H157" s="1"/>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="1"/>
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
@@ -2408,7 +3201,7 @@
       <c r="G158" s="1"/>
       <c r="H158" s="1"/>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="1"/>
       <c r="B159" s="1"/>
       <c r="C159" s="1"/>
@@ -2418,7 +3211,7 @@
       <c r="G159" s="1"/>
       <c r="H159" s="1"/>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="1"/>
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
@@ -2428,7 +3221,7 @@
       <c r="G160" s="1"/>
       <c r="H160" s="1"/>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="1"/>
       <c r="B161" s="1"/>
       <c r="C161" s="1"/>
@@ -2438,7 +3231,7 @@
       <c r="G161" s="1"/>
       <c r="H161" s="1"/>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="1"/>
       <c r="B162" s="1"/>
       <c r="C162" s="1"/>
@@ -2448,7 +3241,7 @@
       <c r="G162" s="1"/>
       <c r="H162" s="1"/>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="1"/>
       <c r="B163" s="1"/>
       <c r="C163" s="1"/>
@@ -2458,7 +3251,7 @@
       <c r="G163" s="1"/>
       <c r="H163" s="1"/>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="1"/>
       <c r="B164" s="1"/>
       <c r="C164" s="1"/>
@@ -2468,7 +3261,7 @@
       <c r="G164" s="1"/>
       <c r="H164" s="1"/>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="1"/>
       <c r="B165" s="1"/>
       <c r="C165" s="1"/>
@@ -2478,7 +3271,7 @@
       <c r="G165" s="1"/>
       <c r="H165" s="1"/>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="1"/>
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
@@ -2488,7 +3281,7 @@
       <c r="G166" s="1"/>
       <c r="H166" s="1"/>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="1"/>
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
@@ -2498,6 +3291,15 @@
       <c r="G167" s="1"/>
       <c r="H167" s="1"/>
     </row>
+    <row r="168" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="169" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="170" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="171" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="172" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="173" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="174" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="175" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="176" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Continuando con el ejercicio de las islas
</commit_message>
<xml_diff>
--- a/MATRICES/matrices.xlsx
+++ b/MATRICES/matrices.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\serve\ARCHIVOS VARIOS\python-exercises\MATRICES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF053F73-560A-4AF7-BDA5-FDD06361AB0C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C316390-A90E-441B-892A-35816CF7E12B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5115" yWindow="3015" windowWidth="15375" windowHeight="7785" xr2:uid="{D8BD301B-0896-44DD-B534-8AC196178EBF}"/>
+    <workbookView xWindow="-21615" yWindow="2880" windowWidth="15375" windowHeight="7785" xr2:uid="{D8BD301B-0896-44DD-B534-8AC196178EBF}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="877" uniqueCount="57">
   <si>
     <t>00</t>
   </si>
@@ -187,6 +187,24 @@
   <si>
     <t>COL</t>
   </si>
+  <si>
+    <t>CASOS</t>
+  </si>
+  <si>
+    <t>100x100</t>
+  </si>
+  <si>
+    <t>p=0</t>
+  </si>
+  <si>
+    <t>p =300</t>
+  </si>
+  <si>
+    <t>p= 200</t>
+  </si>
+  <si>
+    <t>p=100</t>
+  </si>
 </sst>
 </file>
 
@@ -208,7 +226,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -227,6 +245,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -240,7 +282,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -256,6 +298,18 @@
     <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -271,6 +325,1579 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>33130</xdr:colOff>
+      <xdr:row>148</xdr:row>
+      <xdr:rowOff>99391</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>331304</xdr:colOff>
+      <xdr:row>148</xdr:row>
+      <xdr:rowOff>99391</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Conector recto de flecha 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C81E258F-A615-4700-AEA8-CEEF3D3FD413}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="33130" y="28293391"/>
+          <a:ext cx="679174" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>41789</xdr:colOff>
+      <xdr:row>150</xdr:row>
+      <xdr:rowOff>103721</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>339963</xdr:colOff>
+      <xdr:row>150</xdr:row>
+      <xdr:rowOff>103721</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Conector recto de flecha 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{36CD8A36-9727-4899-82DE-A6E67FC12F62}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="41789" y="28678721"/>
+          <a:ext cx="679174" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>20141</xdr:colOff>
+      <xdr:row>151</xdr:row>
+      <xdr:rowOff>121039</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>346364</xdr:colOff>
+      <xdr:row>151</xdr:row>
+      <xdr:rowOff>125557</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Conector recto de flecha 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5454C2E5-24D2-408C-9D83-963AD9E504F4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="20141" y="28886539"/>
+          <a:ext cx="1088223" cy="4518"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>11482</xdr:colOff>
+      <xdr:row>152</xdr:row>
+      <xdr:rowOff>99391</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>346364</xdr:colOff>
+      <xdr:row>152</xdr:row>
+      <xdr:rowOff>108239</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Conector recto de flecha 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11CD752A-EC1F-417E-B507-2ABF8F7704B3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11482" y="29055391"/>
+          <a:ext cx="1477882" cy="8848"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>17318</xdr:colOff>
+      <xdr:row>149</xdr:row>
+      <xdr:rowOff>116898</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>30307</xdr:colOff>
+      <xdr:row>149</xdr:row>
+      <xdr:rowOff>125369</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Conector recto de flecha 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{252A9B82-E80E-4EB0-BFD9-CDBD31655987}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="17318" y="28501398"/>
+          <a:ext cx="393989" cy="8471"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>20141</xdr:colOff>
+      <xdr:row>147</xdr:row>
+      <xdr:rowOff>103909</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>316057</xdr:colOff>
+      <xdr:row>147</xdr:row>
+      <xdr:rowOff>116709</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="14" name="Conector recto de flecha 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7BFADB0D-7F9A-44BB-88DA-C5CC7C17F60B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="20141" y="28107409"/>
+          <a:ext cx="2581916" cy="12800"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>59107</xdr:colOff>
+      <xdr:row>146</xdr:row>
+      <xdr:rowOff>129886</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>355023</xdr:colOff>
+      <xdr:row>146</xdr:row>
+      <xdr:rowOff>142686</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="Conector recto de flecha 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7EC603B6-B4EC-4E75-BEBA-65F778FBCA01}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="59107" y="27942886"/>
+          <a:ext cx="2581916" cy="12800"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>155</xdr:row>
+      <xdr:rowOff>83063</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>196415</xdr:colOff>
+      <xdr:row>158</xdr:row>
+      <xdr:rowOff>5443</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="Conector recto de flecha 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{49BF15B1-180F-406E-A59B-A08F959F9EB6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="571500" y="29610563"/>
+          <a:ext cx="5915" cy="493880"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>172417</xdr:colOff>
+      <xdr:row>155</xdr:row>
+      <xdr:rowOff>32963</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>174171</xdr:colOff>
+      <xdr:row>156</xdr:row>
+      <xdr:rowOff>179614</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="Conector recto de flecha 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C325750-33D8-4087-9F7B-35A352DD6243}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1315417" y="29560463"/>
+          <a:ext cx="1754" cy="337151"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>177983</xdr:colOff>
+      <xdr:row>155</xdr:row>
+      <xdr:rowOff>17625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>195943</xdr:colOff>
+      <xdr:row>158</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="Conector recto de flecha 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{360ED88C-184D-464F-99AB-03B1107BA9BD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2082983" y="29545125"/>
+          <a:ext cx="17960" cy="553875"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>147553</xdr:colOff>
+      <xdr:row>155</xdr:row>
+      <xdr:rowOff>50405</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>168729</xdr:colOff>
+      <xdr:row>161</xdr:row>
+      <xdr:rowOff>157843</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="20" name="Conector recto de flecha 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF3424A6-747B-42C4-82E3-38C4BC5028A6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2433553" y="29577905"/>
+          <a:ext cx="21176" cy="1250438"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>163286</xdr:colOff>
+      <xdr:row>155</xdr:row>
+      <xdr:rowOff>38285</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>169718</xdr:colOff>
+      <xdr:row>157</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="21" name="Conector recto de flecha 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08516F60-0DDC-495B-A117-E5DDBF3C21EC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="925286" y="29565785"/>
+          <a:ext cx="6432" cy="342715"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>188869</xdr:colOff>
+      <xdr:row>155</xdr:row>
+      <xdr:rowOff>73165</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>201385</xdr:colOff>
+      <xdr:row>161</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="22" name="Conector recto de flecha 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00180E20-2CF2-4E4B-A125-EDE3EF5DC1C8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="188869" y="29600665"/>
+          <a:ext cx="12516" cy="1222235"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>174171</xdr:colOff>
+      <xdr:row>155</xdr:row>
+      <xdr:rowOff>16329</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>179615</xdr:colOff>
+      <xdr:row>157</xdr:row>
+      <xdr:rowOff>21771</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="23" name="Conector recto de flecha 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FAB2DBAC-04E8-4B41-8BE7-6A5A44446320}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1698171" y="29543829"/>
+          <a:ext cx="5444" cy="386442"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>370114</xdr:colOff>
+      <xdr:row>166</xdr:row>
+      <xdr:rowOff>108857</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>376030</xdr:colOff>
+      <xdr:row>166</xdr:row>
+      <xdr:rowOff>110277</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="32" name="Conector recto de flecha 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92A9265A-39BE-4A80-84F0-09D3650850CB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="1894114" y="31731857"/>
+          <a:ext cx="767916" cy="1420"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>168</xdr:row>
+      <xdr:rowOff>97971</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>373803</xdr:colOff>
+      <xdr:row>168</xdr:row>
+      <xdr:rowOff>103721</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="33" name="Conector recto de flecha 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28FCEDCE-30B5-4B33-BC54-C7CF9D9DF4E0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="2286000" y="32101971"/>
+          <a:ext cx="373803" cy="5750"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>359229</xdr:colOff>
+      <xdr:row>169</xdr:row>
+      <xdr:rowOff>92529</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>379370</xdr:colOff>
+      <xdr:row>169</xdr:row>
+      <xdr:rowOff>93825</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="34" name="Conector recto de flecha 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A023972-CFF5-486C-A8EB-D3E64FD1E075}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="2264229" y="32287029"/>
+          <a:ext cx="401141" cy="1296"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>5443</xdr:colOff>
+      <xdr:row>170</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>305397</xdr:colOff>
+      <xdr:row>170</xdr:row>
+      <xdr:rowOff>77620</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="35" name="Conector recto de flecha 34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1CA15401-5438-41FB-9427-507DB29CC865}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="1910443" y="32461200"/>
+          <a:ext cx="680954" cy="1420"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>359229</xdr:colOff>
+      <xdr:row>167</xdr:row>
+      <xdr:rowOff>109042</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>6432</xdr:colOff>
+      <xdr:row>167</xdr:row>
+      <xdr:rowOff>119743</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="36" name="Conector recto de flecha 35">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{548ED11B-1192-4716-9900-4AA133775B76}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2264229" y="31922542"/>
+          <a:ext cx="409203" cy="10701"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>5444</xdr:colOff>
+      <xdr:row>165</xdr:row>
+      <xdr:rowOff>119743</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>364671</xdr:colOff>
+      <xdr:row>165</xdr:row>
+      <xdr:rowOff>125186</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="37" name="Conector recto de flecha 36">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E5E5506F-E94A-44B7-B11C-0890BC7E0D39}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="5444" y="31552243"/>
+          <a:ext cx="2645227" cy="5443"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>16329</xdr:colOff>
+      <xdr:row>164</xdr:row>
+      <xdr:rowOff>125186</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>337457</xdr:colOff>
+      <xdr:row>164</xdr:row>
+      <xdr:rowOff>130630</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="38" name="Conector recto de flecha 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5223E0A2-F18A-40D1-9374-2569AE1945CC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="16329" y="31367186"/>
+          <a:ext cx="2607128" cy="5444"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>206829</xdr:colOff>
+      <xdr:row>176</xdr:row>
+      <xdr:rowOff>179614</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>207302</xdr:colOff>
+      <xdr:row>179</xdr:row>
+      <xdr:rowOff>159262</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="50" name="Conector recto de flecha 49">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC19E168-3255-45B7-BA6A-56221CC9F979}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="587829" y="33707614"/>
+          <a:ext cx="473" cy="551148"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>210516</xdr:colOff>
+      <xdr:row>179</xdr:row>
+      <xdr:rowOff>5443</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>212271</xdr:colOff>
+      <xdr:row>180</xdr:row>
+      <xdr:rowOff>185364</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="51" name="Conector recto de flecha 50">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89EC73FF-ED24-4C64-B408-A1AB7A19DF74}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1353516" y="34104943"/>
+          <a:ext cx="1755" cy="370421"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>201386</xdr:colOff>
+      <xdr:row>178</xdr:row>
+      <xdr:rowOff>141515</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>201387</xdr:colOff>
+      <xdr:row>179</xdr:row>
+      <xdr:rowOff>174171</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="52" name="Conector recto de flecha 51">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{667783C7-8C7D-47D2-8D26-F047C4DF7CC9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2106386" y="34050515"/>
+          <a:ext cx="1" cy="223156"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>185655</xdr:colOff>
+      <xdr:row>173</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>201386</xdr:colOff>
+      <xdr:row>180</xdr:row>
+      <xdr:rowOff>28633</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="53" name="Conector recto de flecha 52">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E71B127-5E96-43FF-9590-2BFA691E3782}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2471655" y="32994600"/>
+          <a:ext cx="15731" cy="1324033"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>195943</xdr:colOff>
+      <xdr:row>177</xdr:row>
+      <xdr:rowOff>163286</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>196932</xdr:colOff>
+      <xdr:row>180</xdr:row>
+      <xdr:rowOff>185</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="54" name="Conector recto de flecha 53">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D8BA30F-32B9-481D-AEF7-018776C5B444}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="957943" y="33881786"/>
+          <a:ext cx="989" cy="408399"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>157843</xdr:colOff>
+      <xdr:row>173</xdr:row>
+      <xdr:rowOff>5443</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>183425</xdr:colOff>
+      <xdr:row>180</xdr:row>
+      <xdr:rowOff>18737</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="55" name="Conector recto de flecha 54">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D70DF804-19AD-45A7-AC07-038B8060DD46}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="157843" y="32961943"/>
+          <a:ext cx="25582" cy="1346794"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>190499</xdr:colOff>
+      <xdr:row>180</xdr:row>
+      <xdr:rowOff>10886</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>181</xdr:row>
+      <xdr:rowOff>48986</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="56" name="Conector recto de flecha 55">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DCD9FB84-2031-462A-87AD-008057645C6C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1714499" y="34300886"/>
+          <a:ext cx="1" cy="228600"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -570,10 +2197,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{124D0BB0-B589-4BBF-89A0-F5133410D80B}">
-  <dimension ref="A1:J176"/>
+  <dimension ref="A1:K189"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="192" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A98" sqref="A98:G98"/>
+    <sheetView tabSelected="1" topLeftCell="A138" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I155" sqref="I155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2483,7 +4110,7 @@
       <c r="G96" s="1"/>
       <c r="H96" s="1"/>
     </row>
-    <row r="97" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -2493,7 +4120,7 @@
       <c r="G97" s="1"/>
       <c r="H97" s="1"/>
     </row>
-    <row r="98" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
         <v>0</v>
       </c>
@@ -2517,7 +4144,7 @@
       </c>
       <c r="H98" s="1"/>
     </row>
-    <row r="99" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
         <v>7</v>
       </c>
@@ -2541,7 +4168,7 @@
       </c>
       <c r="H99" s="1"/>
     </row>
-    <row r="100" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
         <v>14</v>
       </c>
@@ -2565,7 +4192,7 @@
       </c>
       <c r="H100" s="1"/>
     </row>
-    <row r="101" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
         <v>21</v>
       </c>
@@ -2589,7 +4216,7 @@
       </c>
       <c r="H101" s="1"/>
     </row>
-    <row r="102" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
         <v>22</v>
       </c>
@@ -2613,7 +4240,7 @@
       </c>
       <c r="H102" s="1"/>
     </row>
-    <row r="103" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
         <v>23</v>
       </c>
@@ -2637,7 +4264,7 @@
       </c>
       <c r="H103" s="1"/>
     </row>
-    <row r="104" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
         <v>24</v>
       </c>
@@ -2661,7 +4288,7 @@
       </c>
       <c r="H104" s="1"/>
     </row>
-    <row r="105" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
@@ -2671,7 +4298,7 @@
       <c r="G105" s="1"/>
       <c r="H105" s="1"/>
     </row>
-    <row r="106" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
@@ -2681,7 +4308,7 @@
       <c r="G106" s="1"/>
       <c r="H106" s="1"/>
     </row>
-    <row r="107" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
@@ -2691,88 +4318,194 @@
       <c r="G107" s="1"/>
       <c r="H107" s="1"/>
     </row>
-    <row r="108" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="1"/>
-      <c r="B108" s="1"/>
-      <c r="C108" s="1"/>
-      <c r="D108" s="1"/>
-      <c r="E108" s="1"/>
-      <c r="F108" s="1"/>
-      <c r="G108" s="1"/>
+    <row r="108" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B108" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C108" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D108" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E108" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F108" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G108" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="H108" s="1"/>
     </row>
-    <row r="109" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="1"/>
-      <c r="B109" s="1"/>
-      <c r="C109" s="1"/>
-      <c r="D109" s="1"/>
-      <c r="E109" s="1"/>
-      <c r="F109" s="1"/>
-      <c r="G109" s="1"/>
+    <row r="109" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B109" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C109" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D109" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E109" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F109" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G109" s="5" t="s">
+        <v>13</v>
+      </c>
       <c r="H109" s="1"/>
     </row>
-    <row r="110" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="1"/>
-      <c r="B110" s="1"/>
-      <c r="C110" s="1"/>
-      <c r="D110" s="1"/>
-      <c r="E110" s="1"/>
-      <c r="F110" s="1"/>
-      <c r="G110" s="1"/>
+    <row r="110" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B110" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C110" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D110" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E110" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F110" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G110" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="H110" s="1"/>
     </row>
-    <row r="111" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="1"/>
-      <c r="B111" s="1"/>
-      <c r="C111" s="1"/>
-      <c r="D111" s="1"/>
-      <c r="E111" s="1"/>
-      <c r="F111" s="1"/>
-      <c r="G111" s="1"/>
+    <row r="111" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B111" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C111" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D111" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E111" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F111" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G111" s="9" t="s">
+        <v>33</v>
+      </c>
       <c r="H111" s="1"/>
-    </row>
-    <row r="112" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="1"/>
-      <c r="B112" s="1"/>
-      <c r="C112" s="1"/>
-      <c r="D112" s="1"/>
-      <c r="E112" s="1"/>
-      <c r="F112" s="1"/>
-      <c r="G112" s="1"/>
+      <c r="I111" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B112" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C112" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D112" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E112" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F112" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G112" s="11" t="s">
+        <v>38</v>
+      </c>
       <c r="H112" s="1"/>
-    </row>
-    <row r="113" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="1"/>
-      <c r="B113" s="1"/>
-      <c r="C113" s="1"/>
-      <c r="D113" s="1"/>
-      <c r="E113" s="1"/>
-      <c r="F113" s="1"/>
-      <c r="G113" s="1"/>
+      <c r="I112" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B113" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C113" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D113" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E113" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F113" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G113" s="9" t="s">
+        <v>43</v>
+      </c>
       <c r="H113" s="1"/>
     </row>
-    <row r="114" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="1"/>
-      <c r="B114" s="1"/>
-      <c r="C114" s="1"/>
-      <c r="D114" s="1"/>
-      <c r="E114" s="1"/>
-      <c r="F114" s="1"/>
-      <c r="G114" s="1"/>
+    <row r="114" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B114" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C114" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D114" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E114" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F114" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="G114" s="5" t="s">
+        <v>30</v>
+      </c>
       <c r="H114" s="1"/>
     </row>
-    <row r="115" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
       <c r="D115" s="1"/>
-      <c r="E115" s="1"/>
+      <c r="E115" s="12"/>
       <c r="F115" s="1"/>
       <c r="G115" s="1"/>
       <c r="H115" s="1"/>
     </row>
-    <row r="116" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="1"/>
+    <row r="116" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
       <c r="D116" s="1"/>
@@ -2781,37 +4514,70 @@
       <c r="G116" s="1"/>
       <c r="H116" s="1"/>
     </row>
-    <row r="117" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="1"/>
-      <c r="B117" s="1"/>
-      <c r="C117" s="1"/>
-      <c r="D117" s="1"/>
+      <c r="B117" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C117" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D117" s="5" t="s">
+        <v>3</v>
+      </c>
       <c r="E117" s="1"/>
       <c r="F117" s="1"/>
       <c r="G117" s="1"/>
       <c r="H117" s="1"/>
     </row>
-    <row r="118" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="1"/>
-      <c r="B118" s="1"/>
-      <c r="C118" s="1"/>
-      <c r="D118" s="1"/>
+      <c r="B118" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C118" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D118" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="E118" s="1"/>
-      <c r="F118" s="1"/>
+      <c r="F118" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="G118" s="1"/>
-      <c r="H118" s="1"/>
-    </row>
-    <row r="119" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H118" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I118" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J118" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K118" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="1"/>
-      <c r="B119" s="1"/>
-      <c r="C119" s="1"/>
-      <c r="D119" s="1"/>
+      <c r="B119" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C119" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D119" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E119" s="1"/>
       <c r="F119" s="1"/>
       <c r="G119" s="1"/>
-      <c r="H119" s="1"/>
-    </row>
-    <row r="120" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H119" s="5"/>
+      <c r="I119" s="5"/>
+      <c r="J119" s="5"/>
+    </row>
+    <row r="120" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
@@ -2819,9 +4585,11 @@
       <c r="E120" s="1"/>
       <c r="F120" s="1"/>
       <c r="G120" s="1"/>
-      <c r="H120" s="1"/>
-    </row>
-    <row r="121" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H120" s="5"/>
+      <c r="I120" s="5"/>
+      <c r="J120" s="5"/>
+    </row>
+    <row r="121" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
@@ -2829,39 +4597,72 @@
       <c r="E121" s="1"/>
       <c r="F121" s="1"/>
       <c r="G121" s="1"/>
-      <c r="H121" s="1"/>
-    </row>
-    <row r="122" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H121" s="5"/>
+      <c r="I121" s="5"/>
+      <c r="J121" s="5"/>
+    </row>
+    <row r="122" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="1"/>
-      <c r="B122" s="1"/>
-      <c r="C122" s="1"/>
-      <c r="D122" s="1"/>
+      <c r="B122" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C122" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D122" s="5" t="s">
+        <v>3</v>
+      </c>
       <c r="E122" s="1"/>
       <c r="F122" s="1"/>
       <c r="G122" s="1"/>
       <c r="H122" s="1"/>
     </row>
-    <row r="123" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="1"/>
-      <c r="B123" s="1"/>
-      <c r="C123" s="1"/>
-      <c r="D123" s="1"/>
+      <c r="B123" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C123" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D123" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="E123" s="1"/>
-      <c r="F123" s="1"/>
+      <c r="F123" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="G123" s="1"/>
-      <c r="H123" s="1"/>
-    </row>
-    <row r="124" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H123" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I123" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J123" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K123" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="1"/>
-      <c r="B124" s="1"/>
-      <c r="C124" s="1"/>
-      <c r="D124" s="1"/>
+      <c r="B124" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C124" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D124" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E124" s="1"/>
       <c r="F124" s="1"/>
       <c r="G124" s="1"/>
       <c r="H124" s="1"/>
     </row>
-    <row r="125" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="1"/>
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
@@ -2871,7 +4672,7 @@
       <c r="G125" s="1"/>
       <c r="H125" s="1"/>
     </row>
-    <row r="126" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="1"/>
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
@@ -2881,37 +4682,68 @@
       <c r="G126" s="1"/>
       <c r="H126" s="1"/>
     </row>
-    <row r="127" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="1"/>
-      <c r="B127" s="1"/>
-      <c r="C127" s="1"/>
-      <c r="D127" s="1"/>
+      <c r="B127" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C127" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D127" s="5" t="s">
+        <v>3</v>
+      </c>
       <c r="E127" s="1"/>
       <c r="F127" s="1"/>
       <c r="G127" s="1"/>
       <c r="H127" s="1"/>
     </row>
-    <row r="128" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="1"/>
-      <c r="B128" s="1"/>
-      <c r="C128" s="1"/>
-      <c r="D128" s="1"/>
+      <c r="B128" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C128" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D128" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="E128" s="1"/>
-      <c r="F128" s="1"/>
+      <c r="F128" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="G128" s="1"/>
-      <c r="H128" s="1"/>
-    </row>
-    <row r="129" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H128" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I128" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J128" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K128" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="1"/>
-      <c r="B129" s="1"/>
-      <c r="C129" s="1"/>
-      <c r="D129" s="1"/>
+      <c r="B129" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C129" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D129" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E129" s="1"/>
       <c r="F129" s="1"/>
       <c r="G129" s="1"/>
       <c r="H129" s="1"/>
     </row>
-    <row r="130" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="1"/>
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
@@ -2921,7 +4753,7 @@
       <c r="G130" s="1"/>
       <c r="H130" s="1"/>
     </row>
-    <row r="131" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="1"/>
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
@@ -2931,37 +4763,65 @@
       <c r="G131" s="1"/>
       <c r="H131" s="1"/>
     </row>
-    <row r="132" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="1"/>
-      <c r="B132" s="1"/>
-      <c r="C132" s="1"/>
-      <c r="D132" s="1"/>
+      <c r="B132" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C132" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D132" s="5" t="s">
+        <v>3</v>
+      </c>
       <c r="E132" s="1"/>
       <c r="F132" s="1"/>
       <c r="G132" s="1"/>
       <c r="H132" s="1"/>
     </row>
-    <row r="133" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="1"/>
-      <c r="B133" s="1"/>
-      <c r="C133" s="1"/>
-      <c r="D133" s="1"/>
+      <c r="B133" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C133" s="7" t="s">
+        <v>9</v>
+      </c>
       <c r="E133" s="1"/>
-      <c r="F133" s="1"/>
+      <c r="F133" s="1" t="s">
+        <v>56</v>
+      </c>
       <c r="G133" s="1"/>
-      <c r="H133" s="1"/>
-    </row>
-    <row r="134" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H133" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I133" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J133" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K133" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="134" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="1"/>
-      <c r="B134" s="1"/>
-      <c r="C134" s="1"/>
-      <c r="D134" s="1"/>
+      <c r="B134" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C134" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D134" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E134" s="1"/>
       <c r="F134" s="1"/>
       <c r="G134" s="1"/>
       <c r="H134" s="1"/>
     </row>
-    <row r="135" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="1"/>
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
@@ -2971,47 +4831,67 @@
       <c r="G135" s="1"/>
       <c r="H135" s="1"/>
     </row>
-    <row r="136" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="1"/>
-      <c r="B136" s="1"/>
-      <c r="C136" s="1"/>
-      <c r="D136" s="1"/>
+    <row r="136" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A136" s="8"/>
+      <c r="B136" s="5"/>
+      <c r="C136" s="5"/>
+      <c r="D136" s="5"/>
       <c r="E136" s="1"/>
       <c r="F136" s="1"/>
       <c r="G136" s="1"/>
       <c r="H136" s="1"/>
     </row>
-    <row r="137" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="1"/>
-      <c r="B137" s="1"/>
-      <c r="C137" s="1"/>
-      <c r="D137" s="1"/>
+    <row r="137" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="8"/>
+      <c r="B137" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C137" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D137" s="9" t="s">
+        <v>29</v>
+      </c>
       <c r="E137" s="1"/>
       <c r="F137" s="1"/>
       <c r="G137" s="1"/>
       <c r="H137" s="1"/>
     </row>
-    <row r="138" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="1"/>
-      <c r="B138" s="1"/>
-      <c r="C138" s="1"/>
-      <c r="D138" s="1"/>
+    <row r="138" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A138" s="8"/>
+      <c r="B138" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C138" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D138" s="9" t="s">
+        <v>48</v>
+      </c>
       <c r="E138" s="1"/>
       <c r="F138" s="1"/>
       <c r="G138" s="1"/>
-      <c r="H138" s="1"/>
-    </row>
-    <row r="139" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H138" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I138" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="J138" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="139" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="1"/>
-      <c r="B139" s="1"/>
-      <c r="C139" s="1"/>
-      <c r="D139" s="1"/>
+      <c r="B139" s="10"/>
+      <c r="C139" s="10"/>
+      <c r="D139" s="10"/>
       <c r="E139" s="1"/>
       <c r="F139" s="1"/>
       <c r="G139" s="1"/>
       <c r="H139" s="1"/>
     </row>
-    <row r="140" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="1"/>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
@@ -3021,7 +4901,7 @@
       <c r="G140" s="1"/>
       <c r="H140" s="1"/>
     </row>
-    <row r="141" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="1"/>
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
@@ -3031,7 +4911,7 @@
       <c r="G141" s="1"/>
       <c r="H141" s="1"/>
     </row>
-    <row r="142" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="1"/>
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
@@ -3041,7 +4921,7 @@
       <c r="G142" s="1"/>
       <c r="H142" s="1"/>
     </row>
-    <row r="143" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="1"/>
       <c r="B143" s="1"/>
       <c r="C143" s="1"/>
@@ -3051,7 +4931,7 @@
       <c r="G143" s="1"/>
       <c r="H143" s="1"/>
     </row>
-    <row r="144" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="1"/>
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
@@ -3082,73 +4962,171 @@
       <c r="H146" s="1"/>
     </row>
     <row r="147" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="1"/>
-      <c r="B147" s="1"/>
-      <c r="C147" s="1"/>
-      <c r="D147" s="1"/>
-      <c r="E147" s="1"/>
-      <c r="F147" s="1"/>
-      <c r="G147" s="1"/>
+      <c r="A147" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B147" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C147" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D147" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E147" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F147" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G147" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="H147" s="1"/>
     </row>
     <row r="148" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="1"/>
-      <c r="B148" s="1"/>
-      <c r="C148" s="1"/>
-      <c r="D148" s="1"/>
-      <c r="E148" s="1"/>
-      <c r="F148" s="1"/>
-      <c r="G148" s="1"/>
+      <c r="A148" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B148" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C148" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D148" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E148" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F148" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G148" s="5" t="s">
+        <v>13</v>
+      </c>
       <c r="H148" s="1"/>
     </row>
     <row r="149" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="1"/>
-      <c r="B149" s="1"/>
-      <c r="C149" s="1"/>
-      <c r="D149" s="1"/>
-      <c r="E149" s="1"/>
-      <c r="F149" s="1"/>
-      <c r="G149" s="1"/>
+      <c r="A149" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B149" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C149" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D149" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E149" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F149" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G149" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="H149" s="1"/>
     </row>
     <row r="150" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="1"/>
-      <c r="B150" s="1"/>
-      <c r="C150" s="1"/>
-      <c r="D150" s="1"/>
-      <c r="E150" s="1"/>
-      <c r="F150" s="1"/>
-      <c r="G150" s="1"/>
+      <c r="A150" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B150" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C150" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D150" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E150" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F150" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G150" s="5" t="s">
+        <v>33</v>
+      </c>
       <c r="H150" s="1"/>
     </row>
     <row r="151" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="1"/>
-      <c r="B151" s="1"/>
-      <c r="C151" s="1"/>
-      <c r="D151" s="1"/>
-      <c r="E151" s="1"/>
-      <c r="F151" s="1"/>
-      <c r="G151" s="1"/>
+      <c r="A151" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B151" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C151" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D151" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E151" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F151" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G151" s="5" t="s">
+        <v>38</v>
+      </c>
       <c r="H151" s="1"/>
     </row>
     <row r="152" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="1"/>
-      <c r="B152" s="1"/>
-      <c r="C152" s="1"/>
-      <c r="D152" s="1"/>
-      <c r="E152" s="1"/>
-      <c r="F152" s="1"/>
-      <c r="G152" s="1"/>
+      <c r="A152" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B152" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C152" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D152" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E152" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F152" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G152" s="5" t="s">
+        <v>43</v>
+      </c>
       <c r="H152" s="1"/>
     </row>
     <row r="153" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="1"/>
-      <c r="B153" s="1"/>
-      <c r="C153" s="1"/>
-      <c r="D153" s="1"/>
-      <c r="E153" s="1"/>
-      <c r="F153" s="1"/>
-      <c r="G153" s="1"/>
+      <c r="A153" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B153" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C153" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D153" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E153" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F153" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G153" s="5" t="s">
+        <v>30</v>
+      </c>
       <c r="H153" s="1"/>
     </row>
     <row r="154" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3172,73 +5150,171 @@
       <c r="H155" s="1"/>
     </row>
     <row r="156" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A156" s="1"/>
-      <c r="B156" s="1"/>
-      <c r="C156" s="1"/>
-      <c r="D156" s="1"/>
-      <c r="E156" s="1"/>
-      <c r="F156" s="1"/>
-      <c r="G156" s="1"/>
+      <c r="A156" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B156" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C156" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D156" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E156" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F156" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G156" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="H156" s="1"/>
     </row>
     <row r="157" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A157" s="1"/>
-      <c r="B157" s="1"/>
-      <c r="C157" s="1"/>
-      <c r="D157" s="1"/>
-      <c r="E157" s="1"/>
-      <c r="F157" s="1"/>
-      <c r="G157" s="1"/>
+      <c r="A157" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B157" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C157" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D157" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E157" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F157" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G157" s="5" t="s">
+        <v>13</v>
+      </c>
       <c r="H157" s="1"/>
     </row>
     <row r="158" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A158" s="1"/>
-      <c r="B158" s="1"/>
-      <c r="C158" s="1"/>
-      <c r="D158" s="1"/>
-      <c r="E158" s="1"/>
-      <c r="F158" s="1"/>
-      <c r="G158" s="1"/>
+      <c r="A158" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B158" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C158" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D158" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E158" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F158" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G158" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="H158" s="1"/>
     </row>
     <row r="159" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A159" s="1"/>
-      <c r="B159" s="1"/>
-      <c r="C159" s="1"/>
-      <c r="D159" s="1"/>
-      <c r="E159" s="1"/>
-      <c r="F159" s="1"/>
-      <c r="G159" s="1"/>
+      <c r="A159" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B159" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C159" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D159" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E159" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F159" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G159" s="5" t="s">
+        <v>33</v>
+      </c>
       <c r="H159" s="1"/>
     </row>
     <row r="160" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A160" s="1"/>
-      <c r="B160" s="1"/>
-      <c r="C160" s="1"/>
-      <c r="D160" s="1"/>
-      <c r="E160" s="1"/>
-      <c r="F160" s="1"/>
-      <c r="G160" s="1"/>
+      <c r="A160" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B160" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C160" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D160" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E160" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F160" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G160" s="5" t="s">
+        <v>38</v>
+      </c>
       <c r="H160" s="1"/>
     </row>
     <row r="161" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A161" s="1"/>
-      <c r="B161" s="1"/>
-      <c r="C161" s="1"/>
-      <c r="D161" s="1"/>
-      <c r="E161" s="1"/>
-      <c r="F161" s="1"/>
-      <c r="G161" s="1"/>
+      <c r="A161" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B161" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C161" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D161" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E161" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F161" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G161" s="5" t="s">
+        <v>43</v>
+      </c>
       <c r="H161" s="1"/>
     </row>
     <row r="162" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A162" s="1"/>
-      <c r="B162" s="1"/>
-      <c r="C162" s="1"/>
-      <c r="D162" s="1"/>
-      <c r="E162" s="1"/>
-      <c r="F162" s="1"/>
-      <c r="G162" s="1"/>
+      <c r="A162" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B162" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C162" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D162" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E162" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F162" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G162" s="5" t="s">
+        <v>30</v>
+      </c>
       <c r="H162" s="1"/>
     </row>
     <row r="163" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3262,49 +5338,499 @@
       <c r="H164" s="1"/>
     </row>
     <row r="165" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A165" s="1"/>
-      <c r="B165" s="1"/>
-      <c r="C165" s="1"/>
-      <c r="D165" s="1"/>
-      <c r="E165" s="1"/>
-      <c r="F165" s="1"/>
-      <c r="G165" s="1"/>
+      <c r="A165" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B165" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C165" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D165" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E165" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F165" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G165" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="H165" s="1"/>
     </row>
     <row r="166" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A166" s="1"/>
-      <c r="B166" s="1"/>
-      <c r="C166" s="1"/>
-      <c r="D166" s="1"/>
-      <c r="E166" s="1"/>
-      <c r="F166" s="1"/>
-      <c r="G166" s="1"/>
+      <c r="A166" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B166" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C166" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D166" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E166" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F166" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G166" s="5" t="s">
+        <v>13</v>
+      </c>
       <c r="H166" s="1"/>
     </row>
     <row r="167" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A167" s="1"/>
-      <c r="B167" s="1"/>
-      <c r="C167" s="1"/>
-      <c r="D167" s="1"/>
-      <c r="E167" s="1"/>
-      <c r="F167" s="1"/>
-      <c r="G167" s="1"/>
+      <c r="A167" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B167" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C167" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D167" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E167" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F167" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G167" s="9" t="s">
+        <v>20</v>
+      </c>
       <c r="H167" s="1"/>
     </row>
-    <row r="168" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="169" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="170" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="171" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="168" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A168" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B168" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C168" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D168" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E168" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F168" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G168" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="169" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A169" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B169" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C169" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D169" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E169" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F169" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G169" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A170" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B170" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C170" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D170" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E170" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F170" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G170" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A171" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B171" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C171" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D171" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E171" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F171" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="G171" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
     <row r="172" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="173" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="174" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="175" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="176" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="174" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A174" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B174" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C174" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D174" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E174" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F174" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G174" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="175" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A175" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B175" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C175" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D175" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E175" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F175" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G175" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="176" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A176" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B176" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C176" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D176" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E176" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F176" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G176" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A177" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B177" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C177" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D177" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E177" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F177" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G177" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A178" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B178" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C178" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D178" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E178" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F178" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G178" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A179" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B179" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C179" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D179" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E179" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F179" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G179" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A180" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B180" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C180" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D180" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E180" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F180" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="G180" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A183" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B183" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C183" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D183" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E183" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F183" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G183" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A184" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B184" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C184" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D184" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E184" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F184" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G184" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A185" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B185" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C185" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D185" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E185" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F185" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G185" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A186" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B186" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C186" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D186" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E186" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F186" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G186" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A187" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B187" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C187" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D187" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E187" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F187" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G187" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A188" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B188" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C188" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D188" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E188" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F188" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G188" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A189" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B189" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C189" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D189" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E189" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F189" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G189" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError sqref="A1:G7" numberStoredAsText="1"/>
   </ignoredErrors>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
EJERCICIO DE ISLAS TERMINADO
</commit_message>
<xml_diff>
--- a/MATRICES/matrices.xlsx
+++ b/MATRICES/matrices.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\serve\ARCHIVOS VARIOS\python-exercises\MATRICES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C316390-A90E-441B-892A-35816CF7E12B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9879379-AB11-4B27-8DD1-C05579220E05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21615" yWindow="2880" windowWidth="15375" windowHeight="7785" xr2:uid="{D8BD301B-0896-44DD-B534-8AC196178EBF}"/>
+    <workbookView xWindow="-28800" yWindow="2685" windowWidth="15375" windowHeight="7785" xr2:uid="{D8BD301B-0896-44DD-B534-8AC196178EBF}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="877" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1039" uniqueCount="58">
   <si>
     <t>00</t>
   </si>
@@ -205,6 +205,9 @@
   <si>
     <t>p=100</t>
   </si>
+  <si>
+    <t xml:space="preserve">FILA-1 ES MENOR QUE </t>
+  </si>
 </sst>
 </file>
 
@@ -226,7 +229,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -269,6 +272,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -282,7 +291,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -310,6 +319,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1676,15 +1694,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>185655</xdr:colOff>
+      <xdr:colOff>185656</xdr:colOff>
       <xdr:row>173</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>21535</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>201386</xdr:colOff>
+      <xdr:colOff>201387</xdr:colOff>
       <xdr:row>180</xdr:row>
-      <xdr:rowOff>28633</xdr:rowOff>
+      <xdr:rowOff>12068</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1699,7 +1717,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="2471655" y="32994600"/>
+          <a:off x="2471656" y="32978035"/>
           <a:ext cx="15731" cy="1324033"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -2197,10 +2215,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{124D0BB0-B589-4BBF-89A0-F5133410D80B}">
-  <dimension ref="A1:K189"/>
+  <dimension ref="A1:K248"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A138" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I155" sqref="I155"/>
+    <sheetView tabSelected="1" topLeftCell="A226" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F238" activeCellId="23" sqref="G239 B239 A239 A238 B236 C237 C236 C235 C234 B234 A234 A233 B233 D235 D236 D237 D238 E238 E237 E235 E236 F236 F237 F238"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4151,13 +4169,13 @@
       <c r="B99" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C99" s="5" t="s">
+      <c r="C99" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D99" s="5" t="s">
+      <c r="D99" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E99" s="5" t="s">
+      <c r="E99" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F99" s="5" t="s">
@@ -4172,19 +4190,19 @@
       <c r="A100" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B100" s="5" t="s">
+      <c r="B100" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C100" s="5" t="s">
+      <c r="C100" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D100" s="5" t="s">
+      <c r="D100" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E100" s="5" t="s">
+      <c r="E100" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F100" s="5" t="s">
+      <c r="F100" s="7" t="s">
         <v>19</v>
       </c>
       <c r="G100" s="5" t="s">
@@ -4193,25 +4211,25 @@
       <c r="H100" s="1"/>
     </row>
     <row r="101" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="5" t="s">
+      <c r="A101" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B101" s="5" t="s">
+      <c r="B101" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C101" s="5" t="s">
+      <c r="C101" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D101" s="5" t="s">
+      <c r="D101" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E101" s="5" t="s">
+      <c r="E101" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F101" s="5" t="s">
+      <c r="F101" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="G101" s="5" t="s">
+      <c r="G101" s="7" t="s">
         <v>33</v>
       </c>
       <c r="H101" s="1"/>
@@ -4220,22 +4238,22 @@
       <c r="A102" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B102" s="5" t="s">
+      <c r="B102" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C102" s="5" t="s">
+      <c r="C102" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D102" s="5" t="s">
+      <c r="D102" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E102" s="5" t="s">
+      <c r="E102" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F102" s="5" t="s">
+      <c r="F102" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="G102" s="5" t="s">
+      <c r="G102" s="7" t="s">
         <v>38</v>
       </c>
       <c r="H102" s="1"/>
@@ -4247,19 +4265,19 @@
       <c r="B103" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C103" s="5" t="s">
+      <c r="C103" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D103" s="5" t="s">
+      <c r="D103" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E103" s="5" t="s">
+      <c r="E103" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F103" s="5" t="s">
+      <c r="F103" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="G103" s="5" t="s">
+      <c r="G103" s="7" t="s">
         <v>43</v>
       </c>
       <c r="H103" s="1"/>
@@ -4277,10 +4295,10 @@
       <c r="D104" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E104" s="5" t="s">
+      <c r="E104" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="F104" s="5" t="s">
+      <c r="F104" s="7" t="s">
         <v>48</v>
       </c>
       <c r="G104" s="5" t="s">
@@ -4293,7 +4311,7 @@
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
       <c r="D105" s="1"/>
-      <c r="E105" s="1"/>
+      <c r="E105" s="12"/>
       <c r="F105" s="1"/>
       <c r="G105" s="1"/>
       <c r="H105" s="1"/>
@@ -5225,7 +5243,7 @@
       <c r="A159" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B159" s="3" t="s">
+      <c r="B159" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C159" s="3" t="s">
@@ -5252,7 +5270,7 @@
       <c r="B160" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C160" s="3" t="s">
+      <c r="C160" s="7" t="s">
         <v>35</v>
       </c>
       <c r="D160" s="3" t="s">
@@ -5279,13 +5297,13 @@
       <c r="C161" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D161" s="3" t="s">
+      <c r="D161" s="7" t="s">
         <v>41</v>
       </c>
       <c r="E161" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F161" s="3" t="s">
+      <c r="F161" s="7" t="s">
         <v>29</v>
       </c>
       <c r="G161" s="5" t="s">
@@ -5306,7 +5324,7 @@
       <c r="D162" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E162" s="3" t="s">
+      <c r="E162" s="7" t="s">
         <v>47</v>
       </c>
       <c r="F162" s="5" t="s">
@@ -5825,6 +5843,621 @@
         <v>30</v>
       </c>
     </row>
+    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A197" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B197" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C197" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D197" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E197" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F197" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G197" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A198" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B198" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C198" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D198" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E198" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F198" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G198" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A199" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B199" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C199" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D199" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E199" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F199" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G199" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A200" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B200" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C200" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D200" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E200" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F200" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G200" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A201" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B201" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C201" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D201" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E201" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F201" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G201" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A202" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B202" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C202" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D202" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E202" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F202" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G202" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A203" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B203" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C203" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D203" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E203" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F203" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G203" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A204" s="1"/>
+      <c r="B204" s="1"/>
+      <c r="C204" s="1"/>
+      <c r="D204" s="1"/>
+      <c r="E204" s="17"/>
+      <c r="F204" s="1"/>
+      <c r="G204" s="1"/>
+    </row>
+    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C208" s="14"/>
+      <c r="F208" s="13"/>
+      <c r="I208" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="209" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B209" s="13"/>
+      <c r="C209" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D209" s="16"/>
+      <c r="E209" s="16"/>
+      <c r="F209" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G209" s="13"/>
+    </row>
+    <row r="210" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
+        <v>49</v>
+      </c>
+      <c r="B210">
+        <v>1</v>
+      </c>
+      <c r="C210" s="16"/>
+      <c r="F210" s="16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="211" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
+        <v>50</v>
+      </c>
+      <c r="B211">
+        <v>-1</v>
+      </c>
+      <c r="F211" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="214" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C214" s="16"/>
+      <c r="F214" s="16"/>
+    </row>
+    <row r="215" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B215" s="13"/>
+      <c r="C215" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D215" s="16"/>
+      <c r="E215" s="16"/>
+      <c r="F215" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G215" s="13"/>
+    </row>
+    <row r="216" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B216" s="15"/>
+      <c r="C216" s="13"/>
+      <c r="F216" s="13"/>
+    </row>
+    <row r="219" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B219" s="16"/>
+    </row>
+    <row r="220" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A220" s="16"/>
+      <c r="B220" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C220" s="16"/>
+      <c r="D220" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="221" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B221" s="13"/>
+      <c r="D221" s="13"/>
+    </row>
+    <row r="224" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B224" s="16"/>
+    </row>
+    <row r="225" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A225" s="13"/>
+      <c r="B225" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C225" s="16"/>
+      <c r="D225" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E225" s="13"/>
+    </row>
+    <row r="226" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B226" s="16"/>
+    </row>
+    <row r="228" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B228" s="13"/>
+      <c r="D228" s="13"/>
+    </row>
+    <row r="229" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A229" s="16"/>
+      <c r="B229" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C229" s="16"/>
+      <c r="D229" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="230" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B230" s="16"/>
+    </row>
+    <row r="232" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A232" s="16"/>
+      <c r="B232" s="16"/>
+    </row>
+    <row r="233" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A233" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B233" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C233" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D233" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E233" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F233" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G233" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="234" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A234" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B234" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C234" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D234" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E234" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F234" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G234" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H234" s="18"/>
+    </row>
+    <row r="235" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A235" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B235" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C235" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D235" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E235" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F235" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G235" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="236" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A236" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B236" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C236" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D236" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E236" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F236" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G236" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="237" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A237" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B237" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C237" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D237" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E237" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F237" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G237" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="238" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A238" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B238" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C238" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D238" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E238" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F238" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G238" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="239" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A239" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B239" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C239" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D239" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E239" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F239" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G239" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="240" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A240" s="16"/>
+      <c r="B240" s="16"/>
+    </row>
+    <row r="242" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A242" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B242" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C242" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D242" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E242" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F242" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G242" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="243" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A243" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B243" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C243" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D243" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E243" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F243" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G243" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="244" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A244" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B244" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C244" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D244" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E244" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F244" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G244" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="245" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A245" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B245" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C245" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D245" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E245" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F245" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G245" s="19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="246" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A246" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B246" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C246" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D246" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E246" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F246" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G246" s="19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="247" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A247" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B247" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C247" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="D247" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E247" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F247" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G247" s="19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="248" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A248" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B248" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C248" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D248" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="E248" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="F248" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="G248" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Ejercicios de Islas, Minimos en filas y columnas, eliminar fila y columna terminados. Empezar ejercicio de censo de poblacion
</commit_message>
<xml_diff>
--- a/MATRICES/matrices.xlsx
+++ b/MATRICES/matrices.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\serve\ARCHIVOS VARIOS\python-exercises\MATRICES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9879379-AB11-4B27-8DD1-C05579220E05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E794782E-F708-4566-BAA6-C884DC30D53D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="2685" windowWidth="15375" windowHeight="7785" xr2:uid="{D8BD301B-0896-44DD-B534-8AC196178EBF}"/>
+    <workbookView xWindow="1125" yWindow="6105" windowWidth="15375" windowHeight="2805" xr2:uid="{D8BD301B-0896-44DD-B534-8AC196178EBF}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1039" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1154" uniqueCount="58">
   <si>
     <t>00</t>
   </si>
@@ -213,7 +213,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -228,8 +228,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -278,8 +284,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -287,11 +299,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -328,6 +355,21 @@
     <xf numFmtId="49" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2215,10 +2257,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{124D0BB0-B589-4BBF-89A0-F5133410D80B}">
-  <dimension ref="A1:K248"/>
+  <dimension ref="A1:K307"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A226" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F238" activeCellId="23" sqref="G239 B239 A239 A238 B236 C237 C236 C235 C234 B234 A234 A233 B233 D235 D236 D237 D238 E238 E237 E235 E236 F236 F237 F238"/>
+    <sheetView tabSelected="1" topLeftCell="A295" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A303" sqref="A303:F303"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6458,6 +6500,1010 @@
         <v>30</v>
       </c>
     </row>
+    <row r="251" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A251" s="16">
+        <v>6</v>
+      </c>
+      <c r="B251" s="20">
+        <v>5</v>
+      </c>
+      <c r="C251" s="16">
+        <v>1</v>
+      </c>
+      <c r="D251" s="16">
+        <v>7</v>
+      </c>
+      <c r="E251" s="16">
+        <v>1</v>
+      </c>
+      <c r="F251" s="16">
+        <v>3</v>
+      </c>
+      <c r="G251" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="252" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A252" s="20">
+        <v>1</v>
+      </c>
+      <c r="B252" s="16">
+        <v>8</v>
+      </c>
+      <c r="C252" s="16">
+        <v>7</v>
+      </c>
+      <c r="D252" s="16">
+        <v>7</v>
+      </c>
+      <c r="E252" s="16">
+        <v>10</v>
+      </c>
+      <c r="F252" s="16">
+        <v>6</v>
+      </c>
+      <c r="G252" s="16">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="253" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A253" s="20">
+        <v>6</v>
+      </c>
+      <c r="B253" s="16">
+        <v>10</v>
+      </c>
+      <c r="C253" s="16">
+        <v>9</v>
+      </c>
+      <c r="D253" s="16">
+        <v>7</v>
+      </c>
+      <c r="E253" s="16">
+        <v>5</v>
+      </c>
+      <c r="F253" s="16">
+        <v>1</v>
+      </c>
+      <c r="G253" s="16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="254" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A254" s="20">
+        <v>6</v>
+      </c>
+      <c r="B254" s="16">
+        <v>1</v>
+      </c>
+      <c r="C254" s="16">
+        <v>8</v>
+      </c>
+      <c r="D254" s="16">
+        <v>8</v>
+      </c>
+      <c r="E254" s="16">
+        <v>1</v>
+      </c>
+      <c r="F254" s="16">
+        <v>5</v>
+      </c>
+      <c r="G254" s="16">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="255" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A255" s="20">
+        <v>9</v>
+      </c>
+      <c r="B255" s="16">
+        <v>6</v>
+      </c>
+      <c r="C255" s="16">
+        <v>6</v>
+      </c>
+      <c r="D255" s="16">
+        <v>5</v>
+      </c>
+      <c r="E255" s="16">
+        <v>1</v>
+      </c>
+      <c r="F255" s="16">
+        <v>2</v>
+      </c>
+      <c r="G255" s="16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="256" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A256" s="20">
+        <v>1</v>
+      </c>
+      <c r="B256" s="16">
+        <v>2</v>
+      </c>
+      <c r="C256" s="16">
+        <v>2</v>
+      </c>
+      <c r="D256" s="16">
+        <v>1</v>
+      </c>
+      <c r="E256" s="16">
+        <v>4</v>
+      </c>
+      <c r="F256" s="16">
+        <v>8</v>
+      </c>
+      <c r="G256" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="257" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A257" s="20">
+        <v>1</v>
+      </c>
+      <c r="B257" s="20">
+        <v>5</v>
+      </c>
+      <c r="C257" s="20">
+        <v>4</v>
+      </c>
+      <c r="D257" s="20">
+        <v>8</v>
+      </c>
+      <c r="E257" s="20">
+        <v>4</v>
+      </c>
+      <c r="F257" s="20">
+        <v>10</v>
+      </c>
+      <c r="G257" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="260" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A260">
+        <v>6</v>
+      </c>
+      <c r="B260">
+        <v>1</v>
+      </c>
+      <c r="C260">
+        <v>7</v>
+      </c>
+      <c r="D260">
+        <v>1</v>
+      </c>
+      <c r="E260">
+        <v>3</v>
+      </c>
+      <c r="F260">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="261" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A261">
+        <v>1</v>
+      </c>
+      <c r="B261">
+        <v>7</v>
+      </c>
+      <c r="C261">
+        <v>7</v>
+      </c>
+      <c r="D261">
+        <v>10</v>
+      </c>
+      <c r="E261">
+        <v>6</v>
+      </c>
+      <c r="F261">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="262" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A262">
+        <v>6</v>
+      </c>
+      <c r="B262">
+        <v>9</v>
+      </c>
+      <c r="C262">
+        <v>7</v>
+      </c>
+      <c r="D262">
+        <v>5</v>
+      </c>
+      <c r="E262">
+        <v>1</v>
+      </c>
+      <c r="F262">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="263" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A263">
+        <v>6</v>
+      </c>
+      <c r="B263">
+        <v>8</v>
+      </c>
+      <c r="C263">
+        <v>8</v>
+      </c>
+      <c r="D263">
+        <v>1</v>
+      </c>
+      <c r="E263">
+        <v>5</v>
+      </c>
+      <c r="F263">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="264" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A264">
+        <v>9</v>
+      </c>
+      <c r="B264">
+        <v>6</v>
+      </c>
+      <c r="C264">
+        <v>5</v>
+      </c>
+      <c r="D264">
+        <v>1</v>
+      </c>
+      <c r="E264">
+        <v>2</v>
+      </c>
+      <c r="F264">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="265" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A265" s="15">
+        <v>1</v>
+      </c>
+      <c r="B265" s="15">
+        <v>2</v>
+      </c>
+      <c r="C265" s="15">
+        <v>1</v>
+      </c>
+      <c r="D265" s="15">
+        <v>4</v>
+      </c>
+      <c r="E265" s="15">
+        <v>8</v>
+      </c>
+      <c r="F265" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="269" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A269" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B269" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C269" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="D269" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E269" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="F269" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="G269" s="21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="270" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A270" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B270" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C270" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="D270" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E270" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="F270" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="G270" s="21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="271" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A271" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B271" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C271" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="D271" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E271" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="F271" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="G271" s="21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="272" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A272" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="B272" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C272" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="D272" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="E272" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="F272" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="G272" s="23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="273" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A273" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B273" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C273" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="D273" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="E273" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="F273" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="G273" s="22" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="274" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A274" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B274" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C274" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="D274" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="E274" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="F274" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="G274" s="22" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="275" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A275" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B275" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C275" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="D275" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="E275" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="F275" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="G275" s="21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="277" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A277" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B277" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C277" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="D277" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="E277" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="F277" s="21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="278" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A278" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B278" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C278" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D278" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E278" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="F278" s="21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="279" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A279" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B279" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C279" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="D279" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="E279" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="F279" s="21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="280" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A280" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B280" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C280" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="D280" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="E280" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="F280" s="22" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="281" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A281" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B281" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C281" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="D281" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="E281" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="F281" s="22" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="282" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A282" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B282" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C282" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="D282" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="E282" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="F282" s="21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="285" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A285">
+        <v>10</v>
+      </c>
+      <c r="B285">
+        <v>3</v>
+      </c>
+      <c r="C285">
+        <v>1</v>
+      </c>
+      <c r="D285">
+        <v>5</v>
+      </c>
+      <c r="E285">
+        <v>9</v>
+      </c>
+      <c r="F285" s="26">
+        <v>3</v>
+      </c>
+      <c r="G285" s="24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="286" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A286">
+        <v>4</v>
+      </c>
+      <c r="B286">
+        <v>3</v>
+      </c>
+      <c r="C286">
+        <v>7</v>
+      </c>
+      <c r="D286">
+        <v>8</v>
+      </c>
+      <c r="E286">
+        <v>4</v>
+      </c>
+      <c r="F286" s="26">
+        <v>4</v>
+      </c>
+      <c r="G286" s="24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="287" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A287">
+        <v>8</v>
+      </c>
+      <c r="B287">
+        <v>2</v>
+      </c>
+      <c r="C287">
+        <v>9</v>
+      </c>
+      <c r="D287">
+        <v>9</v>
+      </c>
+      <c r="E287">
+        <v>9</v>
+      </c>
+      <c r="F287" s="26">
+        <v>4</v>
+      </c>
+      <c r="G287" s="24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="288" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A288" s="26">
+        <v>10</v>
+      </c>
+      <c r="B288" s="26">
+        <v>7</v>
+      </c>
+      <c r="C288" s="26">
+        <v>3</v>
+      </c>
+      <c r="D288" s="26">
+        <v>8</v>
+      </c>
+      <c r="E288" s="26">
+        <v>3</v>
+      </c>
+      <c r="F288" s="26">
+        <v>10</v>
+      </c>
+      <c r="G288" s="25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="289" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A289">
+        <v>4</v>
+      </c>
+      <c r="B289">
+        <v>2</v>
+      </c>
+      <c r="C289">
+        <v>9</v>
+      </c>
+      <c r="D289">
+        <v>5</v>
+      </c>
+      <c r="E289">
+        <v>2</v>
+      </c>
+      <c r="F289" s="26">
+        <v>6</v>
+      </c>
+      <c r="G289" s="24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="290" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A290">
+        <v>7</v>
+      </c>
+      <c r="B290">
+        <v>5</v>
+      </c>
+      <c r="C290">
+        <v>5</v>
+      </c>
+      <c r="D290">
+        <v>10</v>
+      </c>
+      <c r="E290">
+        <v>2</v>
+      </c>
+      <c r="F290" s="26">
+        <v>1</v>
+      </c>
+      <c r="G290" s="24">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="291" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A291">
+        <v>3</v>
+      </c>
+      <c r="B291">
+        <v>8</v>
+      </c>
+      <c r="C291">
+        <v>4</v>
+      </c>
+      <c r="D291">
+        <v>6</v>
+      </c>
+      <c r="E291">
+        <v>2</v>
+      </c>
+      <c r="F291" s="26">
+        <v>4</v>
+      </c>
+      <c r="G291" s="24">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="293" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A293">
+        <v>10</v>
+      </c>
+      <c r="B293">
+        <v>3</v>
+      </c>
+      <c r="C293">
+        <v>1</v>
+      </c>
+      <c r="D293">
+        <v>5</v>
+      </c>
+      <c r="E293">
+        <v>9</v>
+      </c>
+      <c r="F293" s="24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="294" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A294" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B294" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C294" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D294" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E294" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="F294" s="21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="295" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A295" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B295" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C295" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="D295" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="E295" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="F295" s="21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="296" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A296" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B296" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C296" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="D296" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="E296" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="F296" s="22" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="297" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A297" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B297" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C297" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="D297" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="E297" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="F297" s="22" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="298" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A298" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B298" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C298" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="D298" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="E298" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="F298" s="21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="301" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A301" s="15">
+        <v>10</v>
+      </c>
+      <c r="B301" s="15">
+        <v>3</v>
+      </c>
+      <c r="C301" s="15">
+        <v>1</v>
+      </c>
+      <c r="D301" s="15">
+        <v>5</v>
+      </c>
+      <c r="E301" s="15">
+        <v>9</v>
+      </c>
+      <c r="F301" s="15">
+        <v>3</v>
+      </c>
+      <c r="G301" s="28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="302" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A302" s="15">
+        <v>4</v>
+      </c>
+      <c r="B302" s="15">
+        <v>3</v>
+      </c>
+      <c r="C302" s="15">
+        <v>7</v>
+      </c>
+      <c r="D302" s="15">
+        <v>8</v>
+      </c>
+      <c r="E302" s="15">
+        <v>4</v>
+      </c>
+      <c r="F302" s="15">
+        <v>4</v>
+      </c>
+      <c r="G302" s="28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="303" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A303" s="27">
+        <v>8</v>
+      </c>
+      <c r="B303" s="27">
+        <v>2</v>
+      </c>
+      <c r="C303" s="28">
+        <v>9</v>
+      </c>
+      <c r="D303" s="27">
+        <v>9</v>
+      </c>
+      <c r="E303" s="27">
+        <v>9</v>
+      </c>
+      <c r="F303" s="27">
+        <v>4</v>
+      </c>
+      <c r="G303" s="28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="304" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A304" s="15">
+        <v>10</v>
+      </c>
+      <c r="B304" s="15">
+        <v>7</v>
+      </c>
+      <c r="C304" s="15">
+        <v>3</v>
+      </c>
+      <c r="D304" s="15">
+        <v>8</v>
+      </c>
+      <c r="E304" s="15">
+        <v>3</v>
+      </c>
+      <c r="F304" s="15">
+        <v>10</v>
+      </c>
+      <c r="G304" s="28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="305" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A305" s="15">
+        <v>4</v>
+      </c>
+      <c r="B305" s="15">
+        <v>2</v>
+      </c>
+      <c r="C305" s="15">
+        <v>9</v>
+      </c>
+      <c r="D305" s="15">
+        <v>5</v>
+      </c>
+      <c r="E305" s="15">
+        <v>2</v>
+      </c>
+      <c r="F305" s="15">
+        <v>6</v>
+      </c>
+      <c r="G305" s="28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="306" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A306" s="15">
+        <v>7</v>
+      </c>
+      <c r="B306" s="15">
+        <v>5</v>
+      </c>
+      <c r="C306" s="15">
+        <v>5</v>
+      </c>
+      <c r="D306" s="15">
+        <v>10</v>
+      </c>
+      <c r="E306" s="15">
+        <v>2</v>
+      </c>
+      <c r="F306" s="15">
+        <v>1</v>
+      </c>
+      <c r="G306" s="28">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="307" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A307" s="15">
+        <v>3</v>
+      </c>
+      <c r="B307" s="15">
+        <v>8</v>
+      </c>
+      <c r="C307" s="15">
+        <v>4</v>
+      </c>
+      <c r="D307" s="15">
+        <v>6</v>
+      </c>
+      <c r="E307" s="15">
+        <v>2</v>
+      </c>
+      <c r="F307" s="15">
+        <v>4</v>
+      </c>
+      <c r="G307" s="28">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Ejercicios terminados: 16, 17, 18, 19, 20. Por hacer: 21
</commit_message>
<xml_diff>
--- a/MATRICES/matrices.xlsx
+++ b/MATRICES/matrices.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\serve\ARCHIVOS VARIOS\python-exercises\MATRICES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E794782E-F708-4566-BAA6-C884DC30D53D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CF30E5C-06C0-4179-8436-DF40D2F7F2BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="6105" windowWidth="15375" windowHeight="2805" xr2:uid="{D8BD301B-0896-44DD-B534-8AC196178EBF}"/>
+    <workbookView xWindow="-24255" yWindow="-195" windowWidth="21600" windowHeight="11295" xr2:uid="{D8BD301B-0896-44DD-B534-8AC196178EBF}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1154" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1308" uniqueCount="66">
   <si>
     <t>00</t>
   </si>
@@ -208,6 +208,30 @@
   <si>
     <t xml:space="preserve">FILA-1 ES MENOR QUE </t>
   </si>
+  <si>
+    <t>2X10</t>
+  </si>
+  <si>
+    <t>4X6</t>
+  </si>
+  <si>
+    <t>mxn</t>
+  </si>
+  <si>
+    <t>p = 1</t>
+  </si>
+  <si>
+    <t>q = 1</t>
+  </si>
+  <si>
+    <t>07</t>
+  </si>
+  <si>
+    <t>08</t>
+  </si>
+  <si>
+    <t>09</t>
+  </si>
 </sst>
 </file>
 
@@ -235,7 +259,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -290,8 +314,62 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -314,11 +392,55 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -368,8 +490,70 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="17" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="18" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2257,15 +2441,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{124D0BB0-B589-4BBF-89A0-F5133410D80B}">
-  <dimension ref="A1:K307"/>
+  <dimension ref="A1:N406"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A295" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A303" sqref="A303:F303"/>
+    <sheetView tabSelected="1" topLeftCell="A385" zoomScale="134" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H395" sqref="H395"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="7" width="5.7109375" customWidth="1"/>
+    <col min="1" max="24" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7154,7 +7338,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="289" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A289">
         <v>4</v>
       </c>
@@ -7177,7 +7361,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="290" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A290">
         <v>7</v>
       </c>
@@ -7200,7 +7384,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="291" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A291">
         <v>3</v>
       </c>
@@ -7223,7 +7407,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="293" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A293">
         <v>10</v>
       </c>
@@ -7243,7 +7427,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="294" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A294" s="21" t="s">
         <v>7</v>
       </c>
@@ -7263,7 +7447,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="295" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A295" s="21" t="s">
         <v>14</v>
       </c>
@@ -7283,7 +7467,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="296" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A296" s="21" t="s">
         <v>22</v>
       </c>
@@ -7303,7 +7487,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="297" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A297" s="21" t="s">
         <v>23</v>
       </c>
@@ -7323,7 +7507,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="298" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A298" s="21" t="s">
         <v>24</v>
       </c>
@@ -7343,172 +7527,1428 @@
         <v>30</v>
       </c>
     </row>
-    <row r="301" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A301" s="15">
+    <row r="301" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A301" s="32">
         <v>10</v>
       </c>
-      <c r="B301" s="15">
+      <c r="B301" s="33">
         <v>3</v>
       </c>
-      <c r="C301" s="15">
+      <c r="C301" s="36">
         <v>1</v>
       </c>
-      <c r="D301" s="15">
+      <c r="D301" s="37">
         <v>5</v>
       </c>
-      <c r="E301" s="15">
+      <c r="E301" s="40">
         <v>9</v>
       </c>
-      <c r="F301" s="15">
+      <c r="F301" s="41">
         <v>3</v>
       </c>
-      <c r="G301" s="28">
+      <c r="G301" s="27"/>
+      <c r="H301" s="32">
+        <v>10</v>
+      </c>
+      <c r="I301" s="36">
+        <v>1</v>
+      </c>
+      <c r="J301" s="40">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="302" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A302" s="34">
+        <v>4</v>
+      </c>
+      <c r="B302" s="35">
+        <v>3</v>
+      </c>
+      <c r="C302" s="38">
+        <v>7</v>
+      </c>
+      <c r="D302" s="39">
+        <v>8</v>
+      </c>
+      <c r="E302" s="42">
+        <v>4</v>
+      </c>
+      <c r="F302" s="43">
+        <v>4</v>
+      </c>
+      <c r="G302" s="27"/>
+      <c r="H302" s="44">
+        <v>8</v>
+      </c>
+      <c r="I302" s="48">
+        <v>9</v>
+      </c>
+      <c r="J302" s="52">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="303" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A303" s="44">
+        <v>8</v>
+      </c>
+      <c r="B303" s="45">
+        <v>2</v>
+      </c>
+      <c r="C303" s="48">
+        <v>9</v>
+      </c>
+      <c r="D303" s="49">
+        <v>9</v>
+      </c>
+      <c r="E303" s="52">
+        <v>9</v>
+      </c>
+      <c r="F303" s="53">
+        <v>4</v>
+      </c>
+      <c r="G303" s="27"/>
+      <c r="H303" s="56">
+        <v>4</v>
+      </c>
+      <c r="I303" s="60">
+        <v>9</v>
+      </c>
+      <c r="J303" s="64">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="304" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A304" s="46">
+        <v>10</v>
+      </c>
+      <c r="B304" s="47">
+        <v>7</v>
+      </c>
+      <c r="C304" s="50">
+        <v>3</v>
+      </c>
+      <c r="D304" s="51">
+        <v>8</v>
+      </c>
+      <c r="E304" s="54">
+        <v>3</v>
+      </c>
+      <c r="F304" s="55">
+        <v>10</v>
+      </c>
+      <c r="G304" s="27"/>
+    </row>
+    <row r="305" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A305" s="56">
+        <v>4</v>
+      </c>
+      <c r="B305" s="57">
+        <v>2</v>
+      </c>
+      <c r="C305" s="60">
+        <v>9</v>
+      </c>
+      <c r="D305" s="61">
         <v>5</v>
       </c>
-    </row>
-    <row r="302" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A302" s="15">
+      <c r="E305" s="64">
+        <v>2</v>
+      </c>
+      <c r="F305" s="65">
+        <v>6</v>
+      </c>
+      <c r="G305" s="27"/>
+    </row>
+    <row r="306" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A306" s="58">
+        <v>7</v>
+      </c>
+      <c r="B306" s="59">
+        <v>5</v>
+      </c>
+      <c r="C306" s="62">
+        <v>5</v>
+      </c>
+      <c r="D306" s="63">
+        <v>10</v>
+      </c>
+      <c r="E306" s="66">
+        <v>2</v>
+      </c>
+      <c r="F306" s="67">
+        <v>1</v>
+      </c>
+      <c r="G306" s="27"/>
+    </row>
+    <row r="307" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A307" s="15"/>
+      <c r="B307" s="15"/>
+      <c r="C307" s="15"/>
+      <c r="D307" s="15"/>
+      <c r="E307" s="15"/>
+      <c r="F307" s="15"/>
+      <c r="G307" s="27"/>
+    </row>
+    <row r="308" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A308" s="68"/>
+      <c r="B308" s="69"/>
+      <c r="C308" s="68"/>
+      <c r="D308" s="69"/>
+      <c r="E308" s="68"/>
+      <c r="F308" s="69"/>
+      <c r="G308" s="68"/>
+      <c r="H308" s="69"/>
+      <c r="I308" s="28"/>
+      <c r="J308" s="29"/>
+      <c r="M308" t="s">
+        <v>58</v>
+      </c>
+      <c r="N308">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="309" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A309" s="71"/>
+      <c r="B309" s="72"/>
+      <c r="C309" s="71"/>
+      <c r="D309" s="72"/>
+      <c r="E309" s="71"/>
+      <c r="F309" s="72"/>
+      <c r="G309" s="71"/>
+      <c r="H309" s="72"/>
+      <c r="I309" s="30"/>
+      <c r="J309" s="31"/>
+    </row>
+    <row r="311" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A311" s="68"/>
+      <c r="B311" s="69"/>
+      <c r="C311" s="28"/>
+      <c r="D311" s="29"/>
+      <c r="E311" s="68"/>
+      <c r="F311" s="69"/>
+      <c r="G311" s="68"/>
+      <c r="H311" s="69"/>
+    </row>
+    <row r="312" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A312" s="71"/>
+      <c r="B312" s="72"/>
+      <c r="C312" s="30"/>
+      <c r="D312" s="31"/>
+      <c r="E312" s="71"/>
+      <c r="F312" s="72"/>
+      <c r="G312" s="71"/>
+      <c r="H312" s="72"/>
+    </row>
+    <row r="313" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A313" s="68"/>
+      <c r="B313" s="69"/>
+      <c r="C313" s="68"/>
+      <c r="D313" s="69"/>
+      <c r="E313" s="68"/>
+      <c r="F313" s="69"/>
+      <c r="G313" s="68"/>
+      <c r="H313" s="69"/>
+      <c r="M313" t="s">
+        <v>59</v>
+      </c>
+      <c r="N313">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="314" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A314" s="71"/>
+      <c r="B314" s="72"/>
+      <c r="C314" s="71"/>
+      <c r="D314" s="72"/>
+      <c r="E314" s="71"/>
+      <c r="F314" s="72"/>
+      <c r="G314" s="71"/>
+      <c r="H314" s="72"/>
+    </row>
+    <row r="315" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A315" s="70"/>
+      <c r="B315" s="70"/>
+      <c r="C315" s="70"/>
+      <c r="D315" s="70"/>
+      <c r="E315" s="70"/>
+      <c r="F315" s="70"/>
+      <c r="G315" s="70"/>
+      <c r="H315" s="70"/>
+    </row>
+    <row r="317" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A317">
+        <v>5</v>
+      </c>
+      <c r="B317">
+        <v>8</v>
+      </c>
+      <c r="C317">
+        <v>10</v>
+      </c>
+      <c r="D317">
+        <v>3</v>
+      </c>
+      <c r="E317">
+        <v>5</v>
+      </c>
+      <c r="F317">
         <v>4</v>
       </c>
-      <c r="B302" s="15">
+    </row>
+    <row r="318" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A318">
+        <v>9</v>
+      </c>
+      <c r="B318">
+        <v>7</v>
+      </c>
+      <c r="C318">
+        <v>10</v>
+      </c>
+      <c r="D318">
+        <v>6</v>
+      </c>
+      <c r="E318">
+        <v>1</v>
+      </c>
+      <c r="F318">
+        <v>5</v>
+      </c>
+      <c r="I318">
+        <f>A317+A318+B318+B317</f>
+        <v>29</v>
+      </c>
+      <c r="J318">
+        <f>C317+D317+D318+C318</f>
+        <v>29</v>
+      </c>
+      <c r="K318">
+        <f>E317+E318+F318+F317</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="319" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A319">
         <v>3</v>
       </c>
-      <c r="C302" s="15">
+      <c r="B319">
         <v>7</v>
       </c>
-      <c r="D302" s="15">
+      <c r="C319">
+        <v>10</v>
+      </c>
+      <c r="D319">
+        <v>10</v>
+      </c>
+      <c r="E319">
+        <v>3</v>
+      </c>
+      <c r="F319">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="320" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A320">
+        <v>5</v>
+      </c>
+      <c r="B320">
+        <v>1</v>
+      </c>
+      <c r="C320">
+        <v>7</v>
+      </c>
+      <c r="D320">
+        <v>2</v>
+      </c>
+      <c r="E320">
+        <v>3</v>
+      </c>
+      <c r="F320">
+        <v>4</v>
+      </c>
+      <c r="I320">
+        <f>A319+A320+B320+B319</f>
+        <v>16</v>
+      </c>
+      <c r="J320">
+        <f>C319+D319+D320+C320</f>
+        <v>29</v>
+      </c>
+      <c r="K320">
+        <f>E319+E320+F320+F319</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="321" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A321">
+        <v>3</v>
+      </c>
+      <c r="B321">
+        <v>6</v>
+      </c>
+      <c r="C321">
+        <v>10</v>
+      </c>
+      <c r="D321">
+        <v>6</v>
+      </c>
+      <c r="E321">
+        <v>6</v>
+      </c>
+      <c r="F321">
         <v>8</v>
       </c>
-      <c r="E302" s="15">
+    </row>
+    <row r="322" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A322">
         <v>4</v>
       </c>
-      <c r="F302" s="15">
+      <c r="B322">
+        <v>7</v>
+      </c>
+      <c r="C322">
+        <v>9</v>
+      </c>
+      <c r="D322">
+        <v>6</v>
+      </c>
+      <c r="E322">
+        <v>2</v>
+      </c>
+      <c r="F322">
+        <v>10</v>
+      </c>
+      <c r="I322">
+        <f>A321+A322+B322+B321</f>
+        <v>20</v>
+      </c>
+      <c r="J322">
+        <f>C321+D321+D322+C322</f>
+        <v>31</v>
+      </c>
+      <c r="K322">
+        <f>E321+E322+F322+F321</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="325" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A325">
+        <v>483</v>
+      </c>
+      <c r="B325">
+        <v>306</v>
+      </c>
+      <c r="C325">
+        <v>322</v>
+      </c>
+      <c r="D325">
+        <v>940</v>
+      </c>
+      <c r="E325">
         <v>4</v>
       </c>
-      <c r="G302" s="28">
+      <c r="F325">
+        <v>139</v>
+      </c>
+      <c r="G325">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="326" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A326">
+        <v>712</v>
+      </c>
+      <c r="B326">
+        <v>306</v>
+      </c>
+      <c r="C326">
+        <v>313</v>
+      </c>
+      <c r="D326">
+        <v>169</v>
+      </c>
+      <c r="E326">
+        <v>148</v>
+      </c>
+      <c r="F326">
+        <v>503</v>
+      </c>
+      <c r="G326">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="327" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A327">
+        <v>155</v>
+      </c>
+      <c r="B327">
+        <v>127</v>
+      </c>
+      <c r="C327">
+        <v>599</v>
+      </c>
+      <c r="D327">
+        <v>376</v>
+      </c>
+      <c r="E327">
+        <v>279</v>
+      </c>
+      <c r="F327">
+        <v>646</v>
+      </c>
+      <c r="G327">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="328" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A328">
+        <v>773</v>
+      </c>
+      <c r="B328">
+        <v>913</v>
+      </c>
+      <c r="C328">
+        <v>320</v>
+      </c>
+      <c r="D328">
+        <v>184</v>
+      </c>
+      <c r="E328">
+        <v>731</v>
+      </c>
+      <c r="F328">
+        <v>159</v>
+      </c>
+      <c r="G328">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="329" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A329">
+        <v>267</v>
+      </c>
+      <c r="B329">
+        <v>251</v>
+      </c>
+      <c r="C329">
+        <v>493</v>
+      </c>
+      <c r="D329">
+        <v>189</v>
+      </c>
+      <c r="E329">
+        <v>309</v>
+      </c>
+      <c r="F329">
+        <v>361</v>
+      </c>
+      <c r="G329">
+        <v>998</v>
+      </c>
+    </row>
+    <row r="330" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A330">
+        <v>182</v>
+      </c>
+      <c r="B330">
+        <v>277</v>
+      </c>
+      <c r="C330">
+        <v>943</v>
+      </c>
+      <c r="D330">
+        <v>75</v>
+      </c>
+      <c r="E330">
+        <v>444</v>
+      </c>
+      <c r="F330">
+        <v>752</v>
+      </c>
+      <c r="G330">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="331" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A331">
+        <v>434</v>
+      </c>
+      <c r="B331">
+        <v>102</v>
+      </c>
+      <c r="C331">
+        <v>493</v>
+      </c>
+      <c r="D331">
+        <v>990</v>
+      </c>
+      <c r="E331">
+        <v>673</v>
+      </c>
+      <c r="F331">
+        <v>456</v>
+      </c>
+      <c r="G331">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="334" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A334">
+        <v>601</v>
+      </c>
+      <c r="B334">
+        <v>376</v>
+      </c>
+      <c r="C334">
+        <v>444</v>
+      </c>
+      <c r="D334">
+        <v>257</v>
+      </c>
+      <c r="E334">
+        <v>307</v>
+      </c>
+      <c r="F334">
+        <v>516</v>
+      </c>
+      <c r="G334">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="335" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A335">
+        <v>815</v>
+      </c>
+      <c r="B335">
+        <v>143</v>
+      </c>
+      <c r="C335">
+        <v>314</v>
+      </c>
+      <c r="D335">
+        <v>297</v>
+      </c>
+      <c r="E335">
+        <v>761</v>
+      </c>
+      <c r="F335">
+        <v>456</v>
+      </c>
+      <c r="G335">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="336" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A336">
+        <v>985</v>
+      </c>
+      <c r="B336">
+        <v>253</v>
+      </c>
+      <c r="C336">
+        <v>53</v>
+      </c>
+      <c r="D336">
+        <v>936</v>
+      </c>
+      <c r="E336">
+        <v>205</v>
+      </c>
+      <c r="F336">
+        <v>643</v>
+      </c>
+      <c r="G336">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="337" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A337">
+        <v>652</v>
+      </c>
+      <c r="B337">
+        <v>782</v>
+      </c>
+      <c r="C337">
+        <v>397</v>
+      </c>
+      <c r="D337">
+        <v>541</v>
+      </c>
+      <c r="E337">
+        <v>840</v>
+      </c>
+      <c r="F337">
+        <v>384</v>
+      </c>
+      <c r="G337">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="338" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A338">
+        <v>522</v>
+      </c>
+      <c r="B338">
+        <v>41</v>
+      </c>
+      <c r="C338">
+        <v>935</v>
+      </c>
+      <c r="D338">
+        <v>15</v>
+      </c>
+      <c r="E338">
+        <v>877</v>
+      </c>
+      <c r="F338">
+        <v>909</v>
+      </c>
+      <c r="G338">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="339" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A339">
+        <v>243</v>
+      </c>
+      <c r="B339">
+        <v>724</v>
+      </c>
+      <c r="C339">
+        <v>299</v>
+      </c>
+      <c r="D339">
+        <v>714</v>
+      </c>
+      <c r="E339">
+        <v>609</v>
+      </c>
+      <c r="F339">
+        <v>626</v>
+      </c>
+      <c r="G339">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="340" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A340">
+        <v>548</v>
+      </c>
+      <c r="B340">
+        <v>705</v>
+      </c>
+      <c r="C340">
+        <v>202</v>
+      </c>
+      <c r="D340">
+        <v>811</v>
+      </c>
+      <c r="E340">
+        <v>211</v>
+      </c>
+      <c r="F340">
+        <v>347</v>
+      </c>
+      <c r="G340">
+        <v>13</v>
+      </c>
+      <c r="J340">
+        <f>INTERCEPT(A325:G331,A334:G340)</f>
+        <v>402.27501684874215</v>
+      </c>
+    </row>
+    <row r="354" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A354" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B354" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C354" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="D354" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="E354" s="21" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="303" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A303" s="27">
+      <c r="F354" s="21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="355" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A355" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B355" s="75" t="s">
         <v>8</v>
       </c>
-      <c r="B303" s="27">
+      <c r="C355" s="75" t="s">
+        <v>10</v>
+      </c>
+      <c r="D355" s="75" t="s">
+        <v>11</v>
+      </c>
+      <c r="E355" s="75" t="s">
+        <v>12</v>
+      </c>
+      <c r="F355" s="21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="356" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A356" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B356" s="75" t="s">
+        <v>15</v>
+      </c>
+      <c r="C356" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="D356" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="E356" s="75" t="s">
+        <v>19</v>
+      </c>
+      <c r="F356" s="21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="357" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A357" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B357" s="75" t="s">
+        <v>34</v>
+      </c>
+      <c r="C357" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="D357" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="E357" s="75" t="s">
+        <v>37</v>
+      </c>
+      <c r="F357" s="21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="358" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A358" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B358" s="75" t="s">
+        <v>39</v>
+      </c>
+      <c r="C358" s="75" t="s">
+        <v>41</v>
+      </c>
+      <c r="D358" s="75" t="s">
+        <v>42</v>
+      </c>
+      <c r="E358" s="75" t="s">
+        <v>29</v>
+      </c>
+      <c r="F358" s="21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="359" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A359" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B359" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C359" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D359" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="E359" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="F359" s="21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="361" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B361" s="73" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="362" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B362" s="73" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="363" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B363" s="73" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="369" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A369" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B369" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C369" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="D369" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="E369" s="21" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="370" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A370" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B370" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C370" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D370" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E370" s="21" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="371" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A371" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B371" s="74" t="s">
+        <v>15</v>
+      </c>
+      <c r="C371" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="D371" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="E371" s="21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="372" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A372" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B372" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C372" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="D372" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="E372" s="21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="373" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A373" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B373" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C373" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="D373" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="E373" s="21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="380" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A380" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B380" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C380" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="D380" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="E380" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="F380" s="21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="381" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A381" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B381" s="75" t="s">
+        <v>8</v>
+      </c>
+      <c r="C381" s="75" t="s">
+        <v>10</v>
+      </c>
+      <c r="D381" s="75" t="s">
+        <v>11</v>
+      </c>
+      <c r="E381" s="75" t="s">
+        <v>12</v>
+      </c>
+      <c r="F381" s="21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="382" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A382" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B382" s="75" t="s">
+        <v>15</v>
+      </c>
+      <c r="C382" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="D382" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="E382" s="75" t="s">
+        <v>19</v>
+      </c>
+      <c r="F382" s="21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="383" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A383" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B383" s="75" t="s">
+        <v>34</v>
+      </c>
+      <c r="C383" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="D383" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="E383" s="75" t="s">
+        <v>37</v>
+      </c>
+      <c r="F383" s="21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="384" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A384" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B384" s="75" t="s">
+        <v>39</v>
+      </c>
+      <c r="C384" s="75" t="s">
+        <v>41</v>
+      </c>
+      <c r="D384" s="75" t="s">
+        <v>42</v>
+      </c>
+      <c r="E384" s="75" t="s">
+        <v>29</v>
+      </c>
+      <c r="F384" s="21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="385" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A385" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B385" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C385" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D385" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="E385" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="F385" s="21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="386" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A386">
+        <v>70</v>
+      </c>
+      <c r="B386">
+        <v>71</v>
+      </c>
+      <c r="C386">
+        <v>72</v>
+      </c>
+      <c r="D386">
+        <v>73</v>
+      </c>
+      <c r="E386">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="387" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A387">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="388" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A388">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="397" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A397" s="76" t="s">
+        <v>0</v>
+      </c>
+      <c r="B397" s="76" t="s">
+        <v>1</v>
+      </c>
+      <c r="C397" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="C303" s="28">
+      <c r="D397" s="76" t="s">
+        <v>3</v>
+      </c>
+      <c r="E397" s="76" t="s">
+        <v>4</v>
+      </c>
+      <c r="F397" s="76" t="s">
+        <v>5</v>
+      </c>
+      <c r="G397" s="76" t="s">
+        <v>6</v>
+      </c>
+      <c r="H397" s="77" t="s">
+        <v>63</v>
+      </c>
+      <c r="I397" s="77" t="s">
+        <v>64</v>
+      </c>
+      <c r="J397" s="77" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="398" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A398" s="76" t="s">
+        <v>7</v>
+      </c>
+      <c r="B398" s="76" t="s">
+        <v>8</v>
+      </c>
+      <c r="C398" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="D303" s="27">
-        <v>9</v>
-      </c>
-      <c r="E303" s="27">
-        <v>9</v>
-      </c>
-      <c r="F303" s="27">
-        <v>4</v>
-      </c>
-      <c r="G303" s="28">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="304" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A304" s="15">
+      <c r="D398" s="76" t="s">
         <v>10</v>
       </c>
-      <c r="B304" s="15">
-        <v>7</v>
-      </c>
-      <c r="C304" s="15">
-        <v>3</v>
-      </c>
-      <c r="D304" s="15">
-        <v>8</v>
-      </c>
-      <c r="E304" s="15">
-        <v>3</v>
-      </c>
-      <c r="F304" s="15">
-        <v>10</v>
-      </c>
-      <c r="G304" s="28">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="305" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A305" s="15">
-        <v>4</v>
-      </c>
-      <c r="B305" s="15">
-        <v>2</v>
-      </c>
-      <c r="C305" s="15">
-        <v>9</v>
-      </c>
-      <c r="D305" s="15">
-        <v>5</v>
-      </c>
-      <c r="E305" s="15">
-        <v>2</v>
-      </c>
-      <c r="F305" s="15">
-        <v>6</v>
-      </c>
-      <c r="G305" s="28">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="306" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A306" s="15">
-        <v>7</v>
-      </c>
-      <c r="B306" s="15">
-        <v>5</v>
-      </c>
-      <c r="C306" s="15">
-        <v>5</v>
-      </c>
-      <c r="D306" s="15">
-        <v>10</v>
-      </c>
-      <c r="E306" s="15">
-        <v>2</v>
-      </c>
-      <c r="F306" s="15">
-        <v>1</v>
-      </c>
-      <c r="G306" s="28">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="307" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A307" s="15">
-        <v>3</v>
-      </c>
-      <c r="B307" s="15">
-        <v>8</v>
-      </c>
-      <c r="C307" s="15">
-        <v>4</v>
-      </c>
-      <c r="D307" s="15">
-        <v>6</v>
-      </c>
-      <c r="E307" s="15">
-        <v>2</v>
-      </c>
-      <c r="F307" s="15">
-        <v>4</v>
-      </c>
-      <c r="G307" s="28">
-        <v>9</v>
+      <c r="E398" s="76" t="s">
+        <v>11</v>
+      </c>
+      <c r="F398" s="76" t="s">
+        <v>12</v>
+      </c>
+      <c r="G398" s="76" t="s">
+        <v>13</v>
+      </c>
+      <c r="H398" s="77">
+        <v>17</v>
+      </c>
+      <c r="I398" s="77">
+        <v>18</v>
+      </c>
+      <c r="J398" s="77">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="399" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A399" s="78" t="s">
+        <v>14</v>
+      </c>
+      <c r="B399" s="78" t="s">
+        <v>15</v>
+      </c>
+      <c r="C399" s="78" t="s">
+        <v>16</v>
+      </c>
+      <c r="D399" s="78" t="s">
+        <v>17</v>
+      </c>
+      <c r="E399" s="78" t="s">
+        <v>18</v>
+      </c>
+      <c r="F399" s="78" t="s">
+        <v>19</v>
+      </c>
+      <c r="G399" s="78" t="s">
+        <v>20</v>
+      </c>
+      <c r="H399" s="78">
+        <v>27</v>
+      </c>
+      <c r="I399" s="78">
+        <v>28</v>
+      </c>
+      <c r="J399" s="78">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="400" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A400" s="78" t="s">
+        <v>21</v>
+      </c>
+      <c r="B400" s="76" t="s">
+        <v>25</v>
+      </c>
+      <c r="C400" s="76" t="s">
+        <v>26</v>
+      </c>
+      <c r="D400" s="76" t="s">
+        <v>27</v>
+      </c>
+      <c r="E400" s="76" t="s">
+        <v>31</v>
+      </c>
+      <c r="F400" s="76" t="s">
+        <v>32</v>
+      </c>
+      <c r="G400" s="76" t="s">
+        <v>33</v>
+      </c>
+      <c r="H400" s="76">
+        <v>37</v>
+      </c>
+      <c r="I400" s="77">
+        <v>38</v>
+      </c>
+      <c r="J400" s="78">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="401" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A401" s="78" t="s">
+        <v>22</v>
+      </c>
+      <c r="B401" s="76" t="s">
+        <v>34</v>
+      </c>
+      <c r="C401" s="76" t="s">
+        <v>35</v>
+      </c>
+      <c r="D401" s="76" t="s">
+        <v>36</v>
+      </c>
+      <c r="E401" s="76" t="s">
+        <v>28</v>
+      </c>
+      <c r="F401" s="76" t="s">
+        <v>37</v>
+      </c>
+      <c r="G401" s="76" t="s">
+        <v>38</v>
+      </c>
+      <c r="H401" s="76">
+        <v>47</v>
+      </c>
+      <c r="I401" s="77">
+        <v>48</v>
+      </c>
+      <c r="J401" s="78">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="402" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A402" s="78" t="s">
+        <v>23</v>
+      </c>
+      <c r="B402" s="76" t="s">
+        <v>39</v>
+      </c>
+      <c r="C402" s="76" t="s">
+        <v>40</v>
+      </c>
+      <c r="D402" s="76" t="s">
+        <v>41</v>
+      </c>
+      <c r="E402" s="76" t="s">
+        <v>42</v>
+      </c>
+      <c r="F402" s="76" t="s">
+        <v>29</v>
+      </c>
+      <c r="G402" s="76" t="s">
+        <v>43</v>
+      </c>
+      <c r="H402" s="76">
+        <v>57</v>
+      </c>
+      <c r="I402" s="77">
+        <v>58</v>
+      </c>
+      <c r="J402" s="78">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="403" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A403" s="78" t="s">
+        <v>24</v>
+      </c>
+      <c r="B403" s="76" t="s">
+        <v>44</v>
+      </c>
+      <c r="C403" s="76" t="s">
+        <v>45</v>
+      </c>
+      <c r="D403" s="76" t="s">
+        <v>46</v>
+      </c>
+      <c r="E403" s="76" t="s">
+        <v>47</v>
+      </c>
+      <c r="F403" s="76" t="s">
+        <v>48</v>
+      </c>
+      <c r="G403" s="76" t="s">
+        <v>30</v>
+      </c>
+      <c r="H403" s="76">
+        <v>67</v>
+      </c>
+      <c r="I403" s="77">
+        <v>68</v>
+      </c>
+      <c r="J403" s="78">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="404" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A404" s="78">
+        <v>70</v>
+      </c>
+      <c r="B404" s="78">
+        <v>71</v>
+      </c>
+      <c r="C404" s="78">
+        <v>72</v>
+      </c>
+      <c r="D404" s="78">
+        <v>73</v>
+      </c>
+      <c r="E404" s="78">
+        <v>74</v>
+      </c>
+      <c r="F404" s="78">
+        <v>75</v>
+      </c>
+      <c r="G404" s="78">
+        <v>76</v>
+      </c>
+      <c r="H404" s="78">
+        <v>77</v>
+      </c>
+      <c r="I404" s="78">
+        <v>78</v>
+      </c>
+      <c r="J404" s="78">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="405" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A405" s="77">
+        <v>80</v>
+      </c>
+      <c r="B405" s="77">
+        <v>81</v>
+      </c>
+      <c r="C405" s="77">
+        <v>82</v>
+      </c>
+      <c r="D405" s="77">
+        <v>83</v>
+      </c>
+      <c r="E405" s="77">
+        <v>84</v>
+      </c>
+      <c r="F405" s="77">
+        <v>85</v>
+      </c>
+      <c r="G405" s="77">
+        <v>86</v>
+      </c>
+      <c r="H405" s="77">
+        <v>87</v>
+      </c>
+      <c r="I405" s="77">
+        <v>88</v>
+      </c>
+      <c r="J405" s="77">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="406" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A406" s="77">
+        <v>90</v>
+      </c>
+      <c r="B406" s="77">
+        <v>91</v>
+      </c>
+      <c r="C406" s="77">
+        <v>92</v>
+      </c>
+      <c r="D406" s="77">
+        <v>93</v>
+      </c>
+      <c r="E406" s="77">
+        <v>94</v>
+      </c>
+      <c r="F406" s="77">
+        <v>95</v>
+      </c>
+      <c r="G406" s="77">
+        <v>96</v>
+      </c>
+      <c r="H406" s="77">
+        <v>97</v>
+      </c>
+      <c r="I406" s="77">
+        <v>98</v>
+      </c>
+      <c r="J406" s="77">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:G7" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:G7 A397:G403 H397:J397" numberStoredAsText="1"/>
   </ignoredErrors>
   <drawing r:id="rId2"/>
 </worksheet>

</xml_diff>

<commit_message>
Ejercicios practicos terminado. Proyectos sin terminar. Agregar y arreglar README
</commit_message>
<xml_diff>
--- a/MATRICES/matrices.xlsx
+++ b/MATRICES/matrices.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\serve\ARCHIVOS VARIOS\python-exercises\MATRICES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CF30E5C-06C0-4179-8436-DF40D2F7F2BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C93AA30D-366A-4AB1-AA8C-3C0928B3DB28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24255" yWindow="-195" windowWidth="21600" windowHeight="11295" xr2:uid="{D8BD301B-0896-44DD-B534-8AC196178EBF}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1308" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1357" uniqueCount="66">
   <si>
     <t>00</t>
   </si>
@@ -2441,10 +2441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{124D0BB0-B589-4BBF-89A0-F5133410D80B}">
-  <dimension ref="A1:N406"/>
+  <dimension ref="A1:N447"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A385" zoomScale="134" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H395" sqref="H395"/>
+    <sheetView tabSelected="1" topLeftCell="A440" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="I443" sqref="I443"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8944,11 +8944,172 @@
         <v>99</v>
       </c>
     </row>
+    <row r="441" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A441" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B441" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C441" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D441" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E441" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="F441" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="G441" s="21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="442" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A442" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B442" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C442" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="D442" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E442" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="F442" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="G442" s="21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="443" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A443" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B443" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C443" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="D443" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E443" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="F443" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="G443" s="21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="444" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A444" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B444" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C444" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="D444" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E444" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="F444" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="G444" s="21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="445" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A445" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B445" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C445" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="D445" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="E445" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="F445" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="G445" s="21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="446" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A446" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B446" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C446" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="D446" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="E446" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="F446" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="G446" s="21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="447" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A447" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B447" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C447" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="D447" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="E447" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="F447" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="G447" s="21" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:G7 A397:G403 H397:J397" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:G7 A397:G403 H397:J397 A441:G447" numberStoredAsText="1"/>
   </ignoredErrors>
   <drawing r:id="rId2"/>
 </worksheet>

</xml_diff>